<commit_message>
Adaptation du méthaniseur à la couche carbone. Adaptation de la documentation. Adaptation des fichiers exemple. Correction de bugs dans la couche carbone. Fin ajout méthaniseur.
</commit_message>
<xml_diff>
--- a/example/GRAFS_data_example_C.xlsx
+++ b/example/GRAFS_data_example_C.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faustega\Documents\These\isterre-dynamic-modeling\grafs-e-project\grafs-e\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF049BAC-9A74-4EB0-B558-0AA9FF8AF274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E999C94C-9619-4381-B2C7-6308807B731E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
+    <workbookView xWindow="16530" yWindow="-15870" windowWidth="25440" windowHeight="15270" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
   </bookViews>
   <sheets>
     <sheet name="Input data" sheetId="2" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="82">
   <si>
     <t>Area</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Seed input (kt seeds/kt Ymax)</t>
   </si>
   <si>
-    <t>Net Import (ktN)</t>
-  </si>
-  <si>
     <t>Diet</t>
   </si>
   <si>
@@ -282,6 +279,24 @@
   </si>
   <si>
     <t>porcines grasslands excretion</t>
+  </si>
+  <si>
+    <t>Natural meadow forage, Forage</t>
+  </si>
+  <si>
+    <t>Methanizer_diet</t>
+  </si>
+  <si>
+    <t>bovines slurry, bovines manure, porcines slurry, porcines manure</t>
+  </si>
+  <si>
+    <t>waste</t>
+  </si>
+  <si>
+    <t>Barley grain, Wheat grain, Oats grain, Maize corn</t>
+  </si>
+  <si>
+    <t>Methanizer</t>
   </si>
 </sst>
 </file>
@@ -397,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -405,7 +420,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -419,6 +433,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,6 +442,18 @@
   <dxfs count="4">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -480,8 +508,8 @@
     <tableColumn id="3" xr3:uid="{7B352F64-988D-49A0-B664-7D1BD688EE1B}" uniqueName="3" name="Area" queryTableFieldId="3" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{E88EBC76-2C3C-4BE6-B345-902903CB70D2}" uniqueName="4" name="Year" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{C56568E9-7386-48BB-AE51-0A3400CB0D14}" uniqueName="5" name="category" queryTableFieldId="5" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{583513EB-334C-4C54-BF53-D669A066B6B7}" uniqueName="10" name="item" queryTableFieldId="10" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{91174CF9-2FC0-4CE8-B60F-7E15C76A8221}" uniqueName="11" name="value" queryTableFieldId="11" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{583513EB-334C-4C54-BF53-D669A066B6B7}" uniqueName="10" name="item" queryTableFieldId="10" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{91174CF9-2FC0-4CE8-B60F-7E15C76A8221}" uniqueName="11" name="value" queryTableFieldId="11" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -807,8 +835,8 @@
   <dimension ref="A1:E178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E80" sqref="E80"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -838,169 +866,169 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
         <v>1961</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>52</v>
+      <c r="D2" t="s">
+        <v>51</v>
       </c>
       <c r="E2">
         <v>15000</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
         <v>1961</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>53</v>
+      <c r="D3" t="s">
+        <v>52</v>
       </c>
       <c r="E3">
         <v>7500</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
         <v>1961</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>54</v>
+      <c r="D4" t="s">
+        <v>53</v>
       </c>
       <c r="E4">
         <v>2590.69</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>1961</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>55</v>
+      <c r="D5" t="s">
+        <v>54</v>
       </c>
       <c r="E5">
         <v>133.69</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>1961</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>56</v>
+      <c r="D6" t="s">
+        <v>55</v>
       </c>
       <c r="E6">
         <v>25000</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
         <v>1961</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>1961</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="1">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>1961</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>1961</v>
+      </c>
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="1">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>1961</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>65</v>
+      <c r="D9" t="s">
+        <v>64</v>
       </c>
       <c r="E9">
         <v>1448</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10">
         <v>1961</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>66</v>
+      <c r="D10" t="s">
+        <v>65</v>
       </c>
       <c r="E10">
         <v>1188</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="B11">
         <v>1961</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="E11">
@@ -1008,271 +1036,271 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12">
         <v>2023</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12">
+        <v>12143.49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>2023</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="1">
-        <v>12143.49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <v>2023</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13">
+        <v>12834.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>2023</v>
+      </c>
+      <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="1">
-        <v>12834.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14">
-        <v>2023</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14">
+        <v>337.34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>2023</v>
+      </c>
+      <c r="C15" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="1">
-        <v>337.34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15">
-        <v>2023</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="E15">
+        <v>68.27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>2023</v>
+      </c>
+      <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="1">
-        <v>68.27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16">
-        <v>2023</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="E16">
+        <v>35995.57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>2023</v>
+      </c>
+      <c r="C17" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="1">
-        <v>35995.57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17">
-        <v>2023</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="E17">
+        <v>387.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>2023</v>
+      </c>
+      <c r="C18" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="1">
-        <v>387.8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18">
-        <v>2023</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="E18">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>2023</v>
+      </c>
+      <c r="C19" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19">
+        <v>1301.42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>2023</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20">
+        <v>2062.46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>2023</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <v>23882</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>1961</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>2259100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>1961</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19">
-        <v>2023</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1301.42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20">
-        <v>2023</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="1">
-        <v>2062.46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21">
-        <v>2023</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="1">
-        <v>23882</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22">
-        <v>1961</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="E23">
+        <v>980600</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>1961</v>
+      </c>
+      <c r="C24" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="1">
-        <v>2259100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23">
-        <v>1961</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24">
+        <v>1441170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>1961</v>
+      </c>
+      <c r="C25" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="1">
-        <v>980600</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24">
-        <v>1961</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>1961</v>
+      </c>
+      <c r="C26" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="1">
-        <v>1441170</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25">
-        <v>1961</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26">
+        <v>3997300</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>1961</v>
+      </c>
+      <c r="C27" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="1">
-        <v>33000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26">
-        <v>1961</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="1">
-        <v>3997300</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27">
-        <v>1961</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>11</v>
       </c>
       <c r="E27">
@@ -1280,118 +1308,118 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>5</v>
       </c>
       <c r="B28">
         <v>1961</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>22</v>
       </c>
       <c r="E28">
-        <v>5000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>5</v>
       </c>
       <c r="B29">
         <v>2023</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>6</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29">
         <v>1815490</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>5</v>
       </c>
       <c r="B30">
         <v>2023</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E30" s="1">
+      <c r="D30" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30">
         <v>1314680</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>5</v>
       </c>
       <c r="B31">
         <v>2023</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31">
         <v>78900</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>5</v>
       </c>
       <c r="B32">
         <v>2023</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32">
         <v>12120</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>5</v>
       </c>
       <c r="B33">
         <v>2023</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33">
         <v>4998280</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>5</v>
       </c>
       <c r="B34">
         <v>2023</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" t="s">
         <v>11</v>
       </c>
       <c r="E34">
@@ -1399,16 +1427,16 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>5</v>
       </c>
       <c r="B35">
         <v>2023</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" t="s">
         <v>22</v>
       </c>
       <c r="E35">
@@ -1416,220 +1444,220 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>5</v>
       </c>
       <c r="B36">
         <v>1961</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>1961</v>
+      </c>
+      <c r="C37" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" t="s">
         <v>14</v>
       </c>
-      <c r="E36" s="1">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37">
-        <v>1961</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>1961</v>
+      </c>
+      <c r="C38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" t="s">
         <v>14</v>
       </c>
-      <c r="E37" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38">
-        <v>1961</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>1961</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" t="s">
         <v>14</v>
       </c>
-      <c r="E38" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39">
-        <v>1961</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E39" s="1">
+      <c r="E39">
         <v>19501008</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>5</v>
       </c>
       <c r="B40">
         <v>1961</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" t="s">
         <v>68</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="E40">
         <v>46.800000000000004</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>5</v>
       </c>
       <c r="B41">
         <v>1961</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41" s="1" t="s">
+      <c r="C41" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>1961</v>
+      </c>
+      <c r="C42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" t="s">
         <v>70</v>
-      </c>
-      <c r="E41">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B42">
-        <v>1961</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="E42">
         <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>5</v>
       </c>
       <c r="B43">
         <v>1961</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D43" s="1" t="s">
+      <c r="C43" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" t="s">
+        <v>68</v>
+      </c>
+      <c r="E43">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>1961</v>
+      </c>
+      <c r="C44" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" t="s">
         <v>69</v>
       </c>
-      <c r="E43">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B44">
-        <v>1961</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>1961</v>
+      </c>
+      <c r="C45" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45" t="s">
         <v>70</v>
-      </c>
-      <c r="E44">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B45">
-        <v>1961</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="E45">
         <v>0.5</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>5</v>
       </c>
       <c r="B46">
         <v>1961</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>69</v>
+      <c r="C46" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" t="s">
+        <v>68</v>
       </c>
       <c r="E46">
         <v>0.25</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>5</v>
       </c>
       <c r="B47">
         <v>1961</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>70</v>
+      <c r="C47" t="s">
+        <v>71</v>
+      </c>
+      <c r="D47" t="s">
+        <v>69</v>
       </c>
       <c r="E47">
         <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>5</v>
       </c>
       <c r="B48">
         <v>1961</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D48" s="1" t="s">
+      <c r="C48" t="s">
+        <v>47</v>
+      </c>
+      <c r="D48" t="s">
         <v>15</v>
       </c>
       <c r="E48">
@@ -1637,33 +1665,33 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
+      <c r="A49" t="s">
         <v>5</v>
       </c>
       <c r="B49">
         <v>1961</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" t="s">
         <v>16</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" t="s">
         <v>15</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E49">
         <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
         <v>5</v>
       </c>
       <c r="B50">
         <v>1961</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" t="s">
         <v>17</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" t="s">
         <v>15</v>
       </c>
       <c r="E50">
@@ -1671,407 +1699,407 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
+      <c r="A51" t="s">
         <v>5</v>
       </c>
       <c r="B51">
         <v>1961</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>74</v>
+      <c r="C51" t="s">
+        <v>67</v>
+      </c>
+      <c r="D51" t="s">
+        <v>73</v>
       </c>
       <c r="E51">
         <v>35.880000000000003</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
+      <c r="A52" t="s">
         <v>5</v>
       </c>
       <c r="B52">
         <v>1961</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" t="s">
+        <v>67</v>
+      </c>
+      <c r="D52" t="s">
+        <v>74</v>
+      </c>
+      <c r="E52">
+        <v>46.800000000000004</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>1961</v>
+      </c>
+      <c r="C53" t="s">
+        <v>67</v>
+      </c>
+      <c r="D53" t="s">
+        <v>75</v>
+      </c>
+      <c r="E53">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>1961</v>
+      </c>
+      <c r="C54" t="s">
+        <v>72</v>
+      </c>
+      <c r="D54" t="s">
+        <v>73</v>
+      </c>
+      <c r="E54">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55">
+        <v>1961</v>
+      </c>
+      <c r="C55" t="s">
+        <v>72</v>
+      </c>
+      <c r="D55" t="s">
+        <v>74</v>
+      </c>
+      <c r="E55">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <v>1961</v>
+      </c>
+      <c r="C56" t="s">
+        <v>72</v>
+      </c>
+      <c r="D56" t="s">
+        <v>75</v>
+      </c>
+      <c r="E56">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57">
+        <v>1961</v>
+      </c>
+      <c r="C57" t="s">
+        <v>71</v>
+      </c>
+      <c r="D57" t="s">
+        <v>73</v>
+      </c>
+      <c r="E57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58">
+        <v>1961</v>
+      </c>
+      <c r="C58" t="s">
+        <v>71</v>
+      </c>
+      <c r="D58" t="s">
+        <v>74</v>
+      </c>
+      <c r="E58">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59">
+        <v>1961</v>
+      </c>
+      <c r="C59" t="s">
+        <v>71</v>
+      </c>
+      <c r="D59" t="s">
+        <v>75</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60">
+        <v>2023</v>
+      </c>
+      <c r="C60" t="s">
+        <v>47</v>
+      </c>
+      <c r="D60" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61">
+        <v>2023</v>
+      </c>
+      <c r="C61" t="s">
+        <v>16</v>
+      </c>
+      <c r="D61" t="s">
+        <v>14</v>
+      </c>
+      <c r="E61">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62">
+        <v>2023</v>
+      </c>
+      <c r="C62" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" t="s">
+        <v>14</v>
+      </c>
+      <c r="E62">
+        <v>19501008</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63">
+        <v>2023</v>
+      </c>
+      <c r="C63" t="s">
+        <v>67</v>
+      </c>
+      <c r="D63" t="s">
+        <v>70</v>
+      </c>
+      <c r="E63">
+        <v>35.880000000000003</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64">
+        <v>2023</v>
+      </c>
+      <c r="C64" t="s">
+        <v>67</v>
+      </c>
+      <c r="D64" t="s">
         <v>68</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E52" s="1">
-        <v>46.800000000000004</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B53">
-        <v>1961</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E53" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54">
-        <v>1961</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E54" s="1">
-        <v>28.999999999999996</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B55">
-        <v>1961</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E55" s="1">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B56">
-        <v>1961</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E56" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B57">
-        <v>1961</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E57" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B58">
-        <v>1961</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E58" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B59">
-        <v>1961</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E59" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B60">
-        <v>2023</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E60" s="1">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B61">
-        <v>2023</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E61" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B62">
-        <v>2023</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E62" s="1">
-        <v>19501008</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B63">
-        <v>2023</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E63" s="1">
-        <v>35.880000000000003</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B64">
-        <v>2023</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="E64">
         <v>46.800000000000004</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" s="1" t="s">
+      <c r="A65" t="s">
         <v>5</v>
       </c>
       <c r="B65">
         <v>2023</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" t="s">
+        <v>67</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+      <c r="E65">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66">
+        <v>2023</v>
+      </c>
+      <c r="C66" t="s">
+        <v>72</v>
+      </c>
+      <c r="D66" t="s">
+        <v>70</v>
+      </c>
+      <c r="E66">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67">
+        <v>2023</v>
+      </c>
+      <c r="C67" t="s">
+        <v>72</v>
+      </c>
+      <c r="D67" t="s">
         <v>68</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="E67">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68">
+        <v>2023</v>
+      </c>
+      <c r="C68" t="s">
+        <v>72</v>
+      </c>
+      <c r="D68" t="s">
+        <v>69</v>
+      </c>
+      <c r="E68">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69">
+        <v>2023</v>
+      </c>
+      <c r="C69" t="s">
+        <v>71</v>
+      </c>
+      <c r="D69" t="s">
         <v>70</v>
-      </c>
-      <c r="E65">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B66">
-        <v>2023</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E66">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B67">
-        <v>2023</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E67">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B68">
-        <v>2023</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E68">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B69">
-        <v>2023</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="E69">
         <v>0.5</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70" s="1" t="s">
+      <c r="A70" t="s">
         <v>5</v>
       </c>
       <c r="B70">
         <v>2023</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>69</v>
+      <c r="C70" t="s">
+        <v>71</v>
+      </c>
+      <c r="D70" t="s">
+        <v>68</v>
       </c>
       <c r="E70">
         <v>0.25</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" s="1" t="s">
+      <c r="A71" t="s">
         <v>5</v>
       </c>
       <c r="B71">
         <v>2023</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>70</v>
+      <c r="C71" t="s">
+        <v>71</v>
+      </c>
+      <c r="D71" t="s">
+        <v>69</v>
       </c>
       <c r="E71">
         <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72" s="1" t="s">
+      <c r="A72" t="s">
         <v>5</v>
       </c>
       <c r="B72">
         <v>2023</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D72" s="1" t="s">
+      <c r="C72" t="s">
+        <v>47</v>
+      </c>
+      <c r="D72" t="s">
         <v>15</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E72">
         <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" s="1" t="s">
+      <c r="A73" t="s">
         <v>5</v>
       </c>
       <c r="B73">
         <v>2023</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" t="s">
         <v>16</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" t="s">
         <v>15</v>
       </c>
-      <c r="E73" s="1">
+      <c r="E73">
         <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" s="1" t="s">
+      <c r="A74" t="s">
         <v>5</v>
       </c>
       <c r="B74">
         <v>2023</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" t="s">
         <v>17</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D74" t="s">
         <v>15</v>
       </c>
       <c r="E74">
@@ -2079,393 +2107,393 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" s="1" t="s">
+      <c r="A75" t="s">
         <v>5</v>
       </c>
       <c r="B75">
         <v>2023</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>74</v>
+      <c r="C75" t="s">
+        <v>67</v>
+      </c>
+      <c r="D75" t="s">
+        <v>73</v>
       </c>
       <c r="E75">
         <v>35.880000000000003</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A76" s="1" t="s">
+      <c r="A76" t="s">
         <v>5</v>
       </c>
       <c r="B76">
         <v>2023</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D76" s="1" t="s">
+      <c r="C76" t="s">
+        <v>67</v>
+      </c>
+      <c r="D76" t="s">
+        <v>74</v>
+      </c>
+      <c r="E76">
+        <v>46.800000000000004</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77">
+        <v>2023</v>
+      </c>
+      <c r="C77" t="s">
+        <v>67</v>
+      </c>
+      <c r="D77" t="s">
         <v>75</v>
       </c>
-      <c r="E76" s="1">
-        <v>46.800000000000004</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A77" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B77">
-        <v>2023</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E77" s="1">
+      <c r="E77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78">
+        <v>2023</v>
+      </c>
+      <c r="C78" t="s">
+        <v>72</v>
+      </c>
+      <c r="D78" t="s">
+        <v>73</v>
+      </c>
+      <c r="E78">
+        <v>28.999999999999996</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79">
+        <v>2023</v>
+      </c>
+      <c r="C79" t="s">
+        <v>72</v>
+      </c>
+      <c r="D79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>5</v>
+      </c>
+      <c r="B80">
+        <v>2023</v>
+      </c>
+      <c r="C80" t="s">
+        <v>72</v>
+      </c>
+      <c r="D80" t="s">
+        <v>75</v>
+      </c>
+      <c r="E80">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81">
+        <v>2023</v>
+      </c>
+      <c r="C81" t="s">
+        <v>71</v>
+      </c>
+      <c r="D81" t="s">
+        <v>73</v>
+      </c>
+      <c r="E81">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82">
+        <v>2023</v>
+      </c>
+      <c r="C82" t="s">
+        <v>71</v>
+      </c>
+      <c r="D82" t="s">
+        <v>74</v>
+      </c>
+      <c r="E82">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83">
+        <v>2023</v>
+      </c>
+      <c r="C83" t="s">
+        <v>71</v>
+      </c>
+      <c r="D83" t="s">
+        <v>75</v>
+      </c>
+      <c r="E83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84">
+        <v>1961</v>
+      </c>
+      <c r="C84" t="s">
+        <v>18</v>
+      </c>
+      <c r="D84" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84">
+        <v>40000000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85">
+        <v>1961</v>
+      </c>
+      <c r="C85" t="s">
+        <v>48</v>
+      </c>
+      <c r="D85" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E85">
+        <v>11.799999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86">
+        <v>1961</v>
+      </c>
+      <c r="C86" t="s">
+        <v>49</v>
+      </c>
+      <c r="D86" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E86">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87">
+        <v>1961</v>
+      </c>
+      <c r="C87" t="s">
+        <v>50</v>
+      </c>
+      <c r="D87" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E87">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88">
+        <v>1961</v>
+      </c>
+      <c r="C88" t="s">
+        <v>19</v>
+      </c>
+      <c r="D88" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E88">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89">
+        <v>1961</v>
+      </c>
+      <c r="C89" t="s">
+        <v>66</v>
+      </c>
+      <c r="D89" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E89">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90">
+        <v>1961</v>
+      </c>
+      <c r="C90" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A78" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B78">
-        <v>2023</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E78" s="1">
-        <v>28.999999999999996</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B79">
-        <v>2023</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E79" s="1">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A80" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B80">
-        <v>2023</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E80" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A81" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B81">
-        <v>2023</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E81" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A82" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B82">
-        <v>2023</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E82" s="1">
+      <c r="D90" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E90">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91">
+        <v>2023</v>
+      </c>
+      <c r="C91" t="s">
+        <v>18</v>
+      </c>
+      <c r="D91" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E91">
+        <v>70000000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92">
+        <v>2023</v>
+      </c>
+      <c r="C92" t="s">
+        <v>48</v>
+      </c>
+      <c r="D92" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E92">
+        <v>11.799999999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93">
+        <v>2023</v>
+      </c>
+      <c r="C93" t="s">
+        <v>49</v>
+      </c>
+      <c r="D93" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E93">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94">
+        <v>2023</v>
+      </c>
+      <c r="C94" t="s">
+        <v>50</v>
+      </c>
+      <c r="D94" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E94">
         <v>0.2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A83" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B83">
-        <v>2023</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E83" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A84" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B84">
-        <v>1961</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D84" s="5" t="s">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>5</v>
+      </c>
+      <c r="B95">
+        <v>2023</v>
+      </c>
+      <c r="C95" t="s">
+        <v>19</v>
+      </c>
+      <c r="D95" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E84" s="1">
-        <v>40000000</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A85" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B85">
-        <v>1961</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D85" s="6" t="s">
+      <c r="E95">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96">
+        <v>2023</v>
+      </c>
+      <c r="C96" t="s">
+        <v>66</v>
+      </c>
+      <c r="D96" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E85" s="1">
-        <v>11.799999999999999</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A86" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B86">
-        <v>1961</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D86" s="5" t="s">
+      <c r="E96">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97">
+        <v>2023</v>
+      </c>
+      <c r="C97" t="s">
+        <v>20</v>
+      </c>
+      <c r="D97" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E86" s="1">
-        <v>42.5</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A87" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B87">
-        <v>1961</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D87" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E87" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A88" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B88">
-        <v>1961</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E88" s="1">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A89" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B89">
-        <v>1961</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E89" s="1">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A90" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B90">
-        <v>1961</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D90" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E90" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A91" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B91">
-        <v>2023</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E91" s="1">
-        <v>70000000</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A92" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B92">
-        <v>2023</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D92" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E92" s="1">
-        <v>11.799999999999999</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A93" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B93">
-        <v>2023</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D93" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E93" s="1">
-        <v>42.5</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A94" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B94">
-        <v>2023</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D94" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E94" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A95" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B95">
-        <v>2023</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D95" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E95" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A96" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B96">
-        <v>2023</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D96" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E96" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A97" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B97">
-        <v>2023</v>
-      </c>
-      <c r="C97" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E97" s="7">
+      <c r="E97">
         <v>10</v>
       </c>
     </row>
@@ -2497,7 +2525,7 @@
         <v>23</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E99" s="1">
         <v>40</v>
@@ -2616,7 +2644,7 @@
         <v>23</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E106" s="1">
         <v>40</v>
@@ -2735,7 +2763,7 @@
         <v>24</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E113">
         <v>0.03</v>
@@ -2854,7 +2882,7 @@
         <v>24</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E120">
         <v>0.03</v>
@@ -2953,13 +2981,13 @@
         <v>1961</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E126">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
@@ -2970,13 +2998,13 @@
         <v>2023</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E127">
-        <v>150</v>
+        <v>300</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
@@ -2987,13 +3015,13 @@
         <v>1961</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E128">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
@@ -3004,13 +3032,13 @@
         <v>2023</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E129">
-        <v>300</v>
+        <v>70</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
@@ -3021,13 +3049,13 @@
         <v>1961</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E130">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
@@ -3038,13 +3066,13 @@
         <v>2023</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E131">
-        <v>70</v>
+        <v>8</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
@@ -3055,13 +3083,13 @@
         <v>1961</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E132">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
@@ -3069,16 +3097,16 @@
         <v>5</v>
       </c>
       <c r="B133">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E133">
-        <v>8</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
@@ -3086,13 +3114,13 @@
         <v>5</v>
       </c>
       <c r="B134">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E134">
         <v>1</v>
@@ -3103,16 +3131,16 @@
         <v>5</v>
       </c>
       <c r="B135">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E135">
-        <v>10</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
@@ -3123,13 +3151,13 @@
         <v>2023</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E136">
-        <v>1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
@@ -3137,16 +3165,16 @@
         <v>5</v>
       </c>
       <c r="B137">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E137">
-        <v>0.5</v>
+        <v>61</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
@@ -3157,13 +3185,13 @@
         <v>2023</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E138">
-        <v>0.05</v>
+        <v>61</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
@@ -3171,16 +3199,16 @@
         <v>5</v>
       </c>
       <c r="B139">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>63</v>
+        <v>25</v>
+      </c>
+      <c r="D139" t="s">
+        <v>14</v>
+      </c>
+      <c r="E139" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
@@ -3191,13 +3219,13 @@
         <v>2023</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>64</v>
+        <v>25</v>
+      </c>
+      <c r="D140" t="s">
+        <v>15</v>
+      </c>
+      <c r="E140" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
@@ -3208,13 +3236,13 @@
         <v>2023</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D141" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E141" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
@@ -3222,16 +3250,16 @@
         <v>5</v>
       </c>
       <c r="B142">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D142" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E142" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
@@ -3239,16 +3267,16 @@
         <v>5</v>
       </c>
       <c r="B143">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D143" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E143" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
@@ -3259,143 +3287,143 @@
         <v>1961</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D144" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E144" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A145" s="1" t="s">
+      <c r="A145" t="s">
         <v>5</v>
       </c>
       <c r="B145">
         <v>1961</v>
       </c>
-      <c r="C145" s="1" t="s">
-        <v>26</v>
+      <c r="C145" t="s">
+        <v>25</v>
       </c>
       <c r="D145" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="E145" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A146" s="1" t="s">
+      <c r="A146" t="s">
         <v>5</v>
       </c>
       <c r="B146">
-        <v>1961</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>26</v>
+        <v>2023</v>
+      </c>
+      <c r="C146" t="s">
+        <v>25</v>
       </c>
       <c r="D146" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="E146" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A147" s="10" t="s">
+      <c r="A147" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B147" s="2">
         <v>1961</v>
       </c>
       <c r="C147" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D147" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E147" s="8">
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A148" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B148" s="3">
+        <v>1961</v>
+      </c>
+      <c r="C148" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D148" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E148" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A149" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B149" s="2">
+        <v>1961</v>
+      </c>
+      <c r="C149" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="D147" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E147" s="9">
-        <v>2.76</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A148" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B148" s="3">
-        <v>1961</v>
-      </c>
-      <c r="C148" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D148" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E148" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A149" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B149" s="2">
-        <v>1961</v>
-      </c>
-      <c r="C149" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="D149" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E149" s="9">
+      <c r="E149" s="8">
         <v>2.5</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A150" s="11" t="s">
+      <c r="A150" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B150" s="3">
         <v>1961</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E150" s="9">
+        <v>58</v>
+      </c>
+      <c r="E150" s="8">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A151" s="10" t="s">
+      <c r="A151" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B151" s="2">
         <v>1961</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D151" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E151" s="9">
+      <c r="E151" s="8">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A152" s="11" t="s">
+      <c r="A152" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B152" s="3">
         <v>1961</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D152" s="6" t="s">
         <v>8</v>
@@ -3405,116 +3433,116 @@
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A153" s="10" t="s">
+      <c r="A153" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B153" s="2">
         <v>1961</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D153" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E153" s="9">
+      <c r="E153" s="8">
         <v>3.5</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A154" s="11" t="s">
+      <c r="A154" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B154" s="3">
         <v>1961</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D154" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E154" s="12">
+      <c r="E154" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A155" s="10" t="s">
+      <c r="A155" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B155" s="2">
         <v>1961</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D155" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E155" s="13">
+      <c r="E155" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A156" s="10" t="s">
+      <c r="A156" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B156" s="2">
         <v>2023</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D156" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E156" s="9">
+      <c r="E156" s="8">
         <v>2.5</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A157" s="11" t="s">
+      <c r="A157" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B157" s="3">
         <v>2023</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E157" s="9">
+        <v>58</v>
+      </c>
+      <c r="E157" s="8">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A158" s="10" t="s">
+      <c r="A158" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B158" s="2">
         <v>2023</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D158" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E158" s="9">
+      <c r="E158" s="8">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A159" s="11" t="s">
+      <c r="A159" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B159" s="3">
         <v>2023</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D159" s="6" t="s">
         <v>8</v>
@@ -3524,65 +3552,65 @@
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A160" s="10" t="s">
+      <c r="A160" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B160" s="2">
         <v>2023</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D160" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E160" s="9">
+      <c r="E160" s="8">
         <v>3.5</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A161" s="11" t="s">
+      <c r="A161" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B161" s="3">
         <v>2023</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D161" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E161" s="12">
+      <c r="E161" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A162" s="10" t="s">
+      <c r="A162" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B162" s="2">
         <v>2023</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D162" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E162" s="13">
+      <c r="E162" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A163" s="10" t="s">
+      <c r="A163" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B163" s="2">
         <v>1961</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D163" s="5" t="s">
         <v>6</v>
@@ -3592,31 +3620,31 @@
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A164" s="11" t="s">
+      <c r="A164" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B164" s="3">
         <v>1961</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E164">
         <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A165" s="10" t="s">
+      <c r="A165" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B165" s="2">
         <v>1961</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D165" s="5" t="s">
         <v>7</v>
@@ -3626,14 +3654,14 @@
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A166" s="11" t="s">
+      <c r="A166" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B166" s="3">
         <v>1961</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D166" s="6" t="s">
         <v>8</v>
@@ -3643,14 +3671,14 @@
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A167" s="10" t="s">
+      <c r="A167" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B167" s="2">
         <v>1961</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D167" s="5" t="s">
         <v>9</v>
@@ -3660,14 +3688,14 @@
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A168" s="11" t="s">
+      <c r="A168" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B168" s="3">
         <v>1961</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D168" s="6" t="s">
         <v>11</v>
@@ -3677,14 +3705,14 @@
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A169" s="10" t="s">
+      <c r="A169" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B169" s="2">
         <v>1961</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D169" s="5" t="s">
         <v>22</v>
@@ -3694,14 +3722,14 @@
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A170" s="10" t="s">
+      <c r="A170" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B170" s="2">
         <v>2023</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D170" s="5" t="s">
         <v>6</v>
@@ -3711,31 +3739,31 @@
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A171" s="11" t="s">
+      <c r="A171" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B171" s="3">
         <v>2023</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E171">
         <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A172" s="10" t="s">
+      <c r="A172" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B172" s="2">
         <v>2023</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D172" s="5" t="s">
         <v>7</v>
@@ -3745,14 +3773,14 @@
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A173" s="11" t="s">
+      <c r="A173" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B173" s="3">
         <v>2023</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D173" s="6" t="s">
         <v>8</v>
@@ -3762,14 +3790,14 @@
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A174" s="10" t="s">
+      <c r="A174" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B174" s="2">
         <v>2023</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D174" s="5" t="s">
         <v>9</v>
@@ -3779,14 +3807,14 @@
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A175" s="11" t="s">
+      <c r="A175" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B175" s="3">
         <v>2023</v>
       </c>
       <c r="C175" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D175" s="6" t="s">
         <v>11</v>
@@ -3796,14 +3824,14 @@
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A176" s="10" t="s">
+      <c r="A176" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B176" s="2">
         <v>2023</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D176" s="5" t="s">
         <v>22</v>
@@ -3813,34 +3841,34 @@
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A177" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B177" s="15">
-        <v>1961</v>
-      </c>
-      <c r="C177" s="16" t="s">
+      <c r="A177" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B177" s="14">
+        <v>1961</v>
+      </c>
+      <c r="C177" s="15" t="s">
         <v>12</v>
       </c>
       <c r="D177" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E177">
         <v>20</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A178" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B178" s="15">
-        <v>2023</v>
-      </c>
-      <c r="C178" s="16" t="s">
+      <c r="A178" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B178" s="14">
+        <v>2023</v>
+      </c>
+      <c r="C178" s="15" t="s">
         <v>12</v>
       </c>
       <c r="D178" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E178">
         <v>25</v>
@@ -3857,10 +3885,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80ABBC0-87F2-4F7A-9036-33771C52D9AC}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3869,316 +3897,316 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>0.65</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>0.1</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>0.25</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>0.3</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>0.1</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>0.2</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>0.4</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>0.6</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10">
         <v>0.1</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>0.05</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>0.1</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>0.05</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14">
         <v>0.1</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15">
         <v>0.5</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18">
         <v>0.3</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19">
         <v>0.1</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>0.2</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21">
         <v>0.4</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22">
         <v>0.3</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23">
         <v>0.05</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25">
         <v>0.05</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27">
         <v>0.05</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28">
         <v>0.3</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29">
         <v>0.05</v>
@@ -4189,13 +4217,57 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30">
         <v>0.15</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31">
+        <v>0.2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32">
+        <v>0.1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33">
+        <v>0.6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34">
+        <v>0.1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ça fonctionne bien maintenant.
</commit_message>
<xml_diff>
--- a/example/GRAFS_data_example_C.xlsx
+++ b/example/GRAFS_data_example_C.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faustega\Documents\These\isterre-dynamic-modeling\grafs-e-project\grafs-e\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF049BAC-9A74-4EB0-B558-0AA9FF8AF274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E999C94C-9619-4381-B2C7-6308807B731E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
+    <workbookView xWindow="16530" yWindow="-15870" windowWidth="25440" windowHeight="15270" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
   </bookViews>
   <sheets>
     <sheet name="Input data" sheetId="2" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="82">
   <si>
     <t>Area</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Seed input (kt seeds/kt Ymax)</t>
   </si>
   <si>
-    <t>Net Import (ktN)</t>
-  </si>
-  <si>
     <t>Diet</t>
   </si>
   <si>
@@ -282,6 +279,24 @@
   </si>
   <si>
     <t>porcines grasslands excretion</t>
+  </si>
+  <si>
+    <t>Natural meadow forage, Forage</t>
+  </si>
+  <si>
+    <t>Methanizer_diet</t>
+  </si>
+  <si>
+    <t>bovines slurry, bovines manure, porcines slurry, porcines manure</t>
+  </si>
+  <si>
+    <t>waste</t>
+  </si>
+  <si>
+    <t>Barley grain, Wheat grain, Oats grain, Maize corn</t>
+  </si>
+  <si>
+    <t>Methanizer</t>
   </si>
 </sst>
 </file>
@@ -397,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -405,7 +420,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -419,6 +433,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,6 +442,18 @@
   <dxfs count="4">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -480,8 +508,8 @@
     <tableColumn id="3" xr3:uid="{7B352F64-988D-49A0-B664-7D1BD688EE1B}" uniqueName="3" name="Area" queryTableFieldId="3" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{E88EBC76-2C3C-4BE6-B345-902903CB70D2}" uniqueName="4" name="Year" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{C56568E9-7386-48BB-AE51-0A3400CB0D14}" uniqueName="5" name="category" queryTableFieldId="5" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{583513EB-334C-4C54-BF53-D669A066B6B7}" uniqueName="10" name="item" queryTableFieldId="10" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{91174CF9-2FC0-4CE8-B60F-7E15C76A8221}" uniqueName="11" name="value" queryTableFieldId="11" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{583513EB-334C-4C54-BF53-D669A066B6B7}" uniqueName="10" name="item" queryTableFieldId="10" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{91174CF9-2FC0-4CE8-B60F-7E15C76A8221}" uniqueName="11" name="value" queryTableFieldId="11" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -807,8 +835,8 @@
   <dimension ref="A1:E178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E80" sqref="E80"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -838,169 +866,169 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
         <v>1961</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>52</v>
+      <c r="D2" t="s">
+        <v>51</v>
       </c>
       <c r="E2">
         <v>15000</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
         <v>1961</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>53</v>
+      <c r="D3" t="s">
+        <v>52</v>
       </c>
       <c r="E3">
         <v>7500</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
         <v>1961</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>54</v>
+      <c r="D4" t="s">
+        <v>53</v>
       </c>
       <c r="E4">
         <v>2590.69</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>1961</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>55</v>
+      <c r="D5" t="s">
+        <v>54</v>
       </c>
       <c r="E5">
         <v>133.69</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>1961</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>56</v>
+      <c r="D6" t="s">
+        <v>55</v>
       </c>
       <c r="E6">
         <v>25000</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
         <v>1961</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>1961</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="1">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>1961</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>1961</v>
+      </c>
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="1">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>1961</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>65</v>
+      <c r="D9" t="s">
+        <v>64</v>
       </c>
       <c r="E9">
         <v>1448</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10">
         <v>1961</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>66</v>
+      <c r="D10" t="s">
+        <v>65</v>
       </c>
       <c r="E10">
         <v>1188</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="B11">
         <v>1961</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="E11">
@@ -1008,271 +1036,271 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12">
         <v>2023</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12">
+        <v>12143.49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>2023</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="1">
-        <v>12143.49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <v>2023</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13">
+        <v>12834.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>2023</v>
+      </c>
+      <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="1">
-        <v>12834.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14">
-        <v>2023</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14">
+        <v>337.34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>2023</v>
+      </c>
+      <c r="C15" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="1">
-        <v>337.34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15">
-        <v>2023</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="E15">
+        <v>68.27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>2023</v>
+      </c>
+      <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="1">
-        <v>68.27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16">
-        <v>2023</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="E16">
+        <v>35995.57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>2023</v>
+      </c>
+      <c r="C17" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="1">
-        <v>35995.57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17">
-        <v>2023</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="E17">
+        <v>387.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>2023</v>
+      </c>
+      <c r="C18" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="1">
-        <v>387.8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18">
-        <v>2023</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="E18">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>2023</v>
+      </c>
+      <c r="C19" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19">
+        <v>1301.42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>2023</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20">
+        <v>2062.46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>2023</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <v>23882</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>1961</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>2259100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>1961</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19">
-        <v>2023</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1301.42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20">
-        <v>2023</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="1">
-        <v>2062.46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21">
-        <v>2023</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="1">
-        <v>23882</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22">
-        <v>1961</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="E23">
+        <v>980600</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>1961</v>
+      </c>
+      <c r="C24" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="1">
-        <v>2259100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23">
-        <v>1961</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24">
+        <v>1441170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>1961</v>
+      </c>
+      <c r="C25" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="1">
-        <v>980600</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24">
-        <v>1961</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>1961</v>
+      </c>
+      <c r="C26" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="1">
-        <v>1441170</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25">
-        <v>1961</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26">
+        <v>3997300</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>1961</v>
+      </c>
+      <c r="C27" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="1">
-        <v>33000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26">
-        <v>1961</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="1">
-        <v>3997300</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27">
-        <v>1961</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>11</v>
       </c>
       <c r="E27">
@@ -1280,118 +1308,118 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>5</v>
       </c>
       <c r="B28">
         <v>1961</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>22</v>
       </c>
       <c r="E28">
-        <v>5000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>5</v>
       </c>
       <c r="B29">
         <v>2023</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>6</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29">
         <v>1815490</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>5</v>
       </c>
       <c r="B30">
         <v>2023</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E30" s="1">
+      <c r="D30" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30">
         <v>1314680</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>5</v>
       </c>
       <c r="B31">
         <v>2023</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31">
         <v>78900</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>5</v>
       </c>
       <c r="B32">
         <v>2023</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32">
         <v>12120</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>5</v>
       </c>
       <c r="B33">
         <v>2023</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33">
         <v>4998280</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>5</v>
       </c>
       <c r="B34">
         <v>2023</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" t="s">
         <v>11</v>
       </c>
       <c r="E34">
@@ -1399,16 +1427,16 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>5</v>
       </c>
       <c r="B35">
         <v>2023</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" t="s">
         <v>22</v>
       </c>
       <c r="E35">
@@ -1416,220 +1444,220 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>5</v>
       </c>
       <c r="B36">
         <v>1961</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>1961</v>
+      </c>
+      <c r="C37" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" t="s">
         <v>14</v>
       </c>
-      <c r="E36" s="1">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37">
-        <v>1961</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>1961</v>
+      </c>
+      <c r="C38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" t="s">
         <v>14</v>
       </c>
-      <c r="E37" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38">
-        <v>1961</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>1961</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" t="s">
         <v>14</v>
       </c>
-      <c r="E38" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39">
-        <v>1961</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E39" s="1">
+      <c r="E39">
         <v>19501008</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>5</v>
       </c>
       <c r="B40">
         <v>1961</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" t="s">
         <v>68</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="E40">
         <v>46.800000000000004</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>5</v>
       </c>
       <c r="B41">
         <v>1961</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41" s="1" t="s">
+      <c r="C41" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>1961</v>
+      </c>
+      <c r="C42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" t="s">
         <v>70</v>
-      </c>
-      <c r="E41">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B42">
-        <v>1961</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="E42">
         <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>5</v>
       </c>
       <c r="B43">
         <v>1961</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D43" s="1" t="s">
+      <c r="C43" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" t="s">
+        <v>68</v>
+      </c>
+      <c r="E43">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>1961</v>
+      </c>
+      <c r="C44" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" t="s">
         <v>69</v>
       </c>
-      <c r="E43">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B44">
-        <v>1961</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>1961</v>
+      </c>
+      <c r="C45" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45" t="s">
         <v>70</v>
-      </c>
-      <c r="E44">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B45">
-        <v>1961</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="E45">
         <v>0.5</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>5</v>
       </c>
       <c r="B46">
         <v>1961</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>69</v>
+      <c r="C46" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" t="s">
+        <v>68</v>
       </c>
       <c r="E46">
         <v>0.25</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>5</v>
       </c>
       <c r="B47">
         <v>1961</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>70</v>
+      <c r="C47" t="s">
+        <v>71</v>
+      </c>
+      <c r="D47" t="s">
+        <v>69</v>
       </c>
       <c r="E47">
         <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>5</v>
       </c>
       <c r="B48">
         <v>1961</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D48" s="1" t="s">
+      <c r="C48" t="s">
+        <v>47</v>
+      </c>
+      <c r="D48" t="s">
         <v>15</v>
       </c>
       <c r="E48">
@@ -1637,33 +1665,33 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
+      <c r="A49" t="s">
         <v>5</v>
       </c>
       <c r="B49">
         <v>1961</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" t="s">
         <v>16</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" t="s">
         <v>15</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E49">
         <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
         <v>5</v>
       </c>
       <c r="B50">
         <v>1961</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" t="s">
         <v>17</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" t="s">
         <v>15</v>
       </c>
       <c r="E50">
@@ -1671,407 +1699,407 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
+      <c r="A51" t="s">
         <v>5</v>
       </c>
       <c r="B51">
         <v>1961</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>74</v>
+      <c r="C51" t="s">
+        <v>67</v>
+      </c>
+      <c r="D51" t="s">
+        <v>73</v>
       </c>
       <c r="E51">
         <v>35.880000000000003</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
+      <c r="A52" t="s">
         <v>5</v>
       </c>
       <c r="B52">
         <v>1961</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" t="s">
+        <v>67</v>
+      </c>
+      <c r="D52" t="s">
+        <v>74</v>
+      </c>
+      <c r="E52">
+        <v>46.800000000000004</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>1961</v>
+      </c>
+      <c r="C53" t="s">
+        <v>67</v>
+      </c>
+      <c r="D53" t="s">
+        <v>75</v>
+      </c>
+      <c r="E53">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>1961</v>
+      </c>
+      <c r="C54" t="s">
+        <v>72</v>
+      </c>
+      <c r="D54" t="s">
+        <v>73</v>
+      </c>
+      <c r="E54">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55">
+        <v>1961</v>
+      </c>
+      <c r="C55" t="s">
+        <v>72</v>
+      </c>
+      <c r="D55" t="s">
+        <v>74</v>
+      </c>
+      <c r="E55">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <v>1961</v>
+      </c>
+      <c r="C56" t="s">
+        <v>72</v>
+      </c>
+      <c r="D56" t="s">
+        <v>75</v>
+      </c>
+      <c r="E56">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57">
+        <v>1961</v>
+      </c>
+      <c r="C57" t="s">
+        <v>71</v>
+      </c>
+      <c r="D57" t="s">
+        <v>73</v>
+      </c>
+      <c r="E57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58">
+        <v>1961</v>
+      </c>
+      <c r="C58" t="s">
+        <v>71</v>
+      </c>
+      <c r="D58" t="s">
+        <v>74</v>
+      </c>
+      <c r="E58">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59">
+        <v>1961</v>
+      </c>
+      <c r="C59" t="s">
+        <v>71</v>
+      </c>
+      <c r="D59" t="s">
+        <v>75</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60">
+        <v>2023</v>
+      </c>
+      <c r="C60" t="s">
+        <v>47</v>
+      </c>
+      <c r="D60" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61">
+        <v>2023</v>
+      </c>
+      <c r="C61" t="s">
+        <v>16</v>
+      </c>
+      <c r="D61" t="s">
+        <v>14</v>
+      </c>
+      <c r="E61">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62">
+        <v>2023</v>
+      </c>
+      <c r="C62" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" t="s">
+        <v>14</v>
+      </c>
+      <c r="E62">
+        <v>19501008</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63">
+        <v>2023</v>
+      </c>
+      <c r="C63" t="s">
+        <v>67</v>
+      </c>
+      <c r="D63" t="s">
+        <v>70</v>
+      </c>
+      <c r="E63">
+        <v>35.880000000000003</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64">
+        <v>2023</v>
+      </c>
+      <c r="C64" t="s">
+        <v>67</v>
+      </c>
+      <c r="D64" t="s">
         <v>68</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E52" s="1">
-        <v>46.800000000000004</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B53">
-        <v>1961</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E53" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54">
-        <v>1961</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E54" s="1">
-        <v>28.999999999999996</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B55">
-        <v>1961</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E55" s="1">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B56">
-        <v>1961</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E56" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B57">
-        <v>1961</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E57" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B58">
-        <v>1961</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E58" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B59">
-        <v>1961</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E59" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B60">
-        <v>2023</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E60" s="1">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B61">
-        <v>2023</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E61" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B62">
-        <v>2023</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E62" s="1">
-        <v>19501008</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B63">
-        <v>2023</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E63" s="1">
-        <v>35.880000000000003</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B64">
-        <v>2023</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="E64">
         <v>46.800000000000004</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" s="1" t="s">
+      <c r="A65" t="s">
         <v>5</v>
       </c>
       <c r="B65">
         <v>2023</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" t="s">
+        <v>67</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+      <c r="E65">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66">
+        <v>2023</v>
+      </c>
+      <c r="C66" t="s">
+        <v>72</v>
+      </c>
+      <c r="D66" t="s">
+        <v>70</v>
+      </c>
+      <c r="E66">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67">
+        <v>2023</v>
+      </c>
+      <c r="C67" t="s">
+        <v>72</v>
+      </c>
+      <c r="D67" t="s">
         <v>68</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="E67">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68">
+        <v>2023</v>
+      </c>
+      <c r="C68" t="s">
+        <v>72</v>
+      </c>
+      <c r="D68" t="s">
+        <v>69</v>
+      </c>
+      <c r="E68">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69">
+        <v>2023</v>
+      </c>
+      <c r="C69" t="s">
+        <v>71</v>
+      </c>
+      <c r="D69" t="s">
         <v>70</v>
-      </c>
-      <c r="E65">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B66">
-        <v>2023</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E66">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B67">
-        <v>2023</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E67">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B68">
-        <v>2023</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E68">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B69">
-        <v>2023</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="E69">
         <v>0.5</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70" s="1" t="s">
+      <c r="A70" t="s">
         <v>5</v>
       </c>
       <c r="B70">
         <v>2023</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>69</v>
+      <c r="C70" t="s">
+        <v>71</v>
+      </c>
+      <c r="D70" t="s">
+        <v>68</v>
       </c>
       <c r="E70">
         <v>0.25</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" s="1" t="s">
+      <c r="A71" t="s">
         <v>5</v>
       </c>
       <c r="B71">
         <v>2023</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>70</v>
+      <c r="C71" t="s">
+        <v>71</v>
+      </c>
+      <c r="D71" t="s">
+        <v>69</v>
       </c>
       <c r="E71">
         <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72" s="1" t="s">
+      <c r="A72" t="s">
         <v>5</v>
       </c>
       <c r="B72">
         <v>2023</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D72" s="1" t="s">
+      <c r="C72" t="s">
+        <v>47</v>
+      </c>
+      <c r="D72" t="s">
         <v>15</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E72">
         <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" s="1" t="s">
+      <c r="A73" t="s">
         <v>5</v>
       </c>
       <c r="B73">
         <v>2023</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" t="s">
         <v>16</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" t="s">
         <v>15</v>
       </c>
-      <c r="E73" s="1">
+      <c r="E73">
         <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" s="1" t="s">
+      <c r="A74" t="s">
         <v>5</v>
       </c>
       <c r="B74">
         <v>2023</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" t="s">
         <v>17</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D74" t="s">
         <v>15</v>
       </c>
       <c r="E74">
@@ -2079,393 +2107,393 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" s="1" t="s">
+      <c r="A75" t="s">
         <v>5</v>
       </c>
       <c r="B75">
         <v>2023</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>74</v>
+      <c r="C75" t="s">
+        <v>67</v>
+      </c>
+      <c r="D75" t="s">
+        <v>73</v>
       </c>
       <c r="E75">
         <v>35.880000000000003</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A76" s="1" t="s">
+      <c r="A76" t="s">
         <v>5</v>
       </c>
       <c r="B76">
         <v>2023</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D76" s="1" t="s">
+      <c r="C76" t="s">
+        <v>67</v>
+      </c>
+      <c r="D76" t="s">
+        <v>74</v>
+      </c>
+      <c r="E76">
+        <v>46.800000000000004</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77">
+        <v>2023</v>
+      </c>
+      <c r="C77" t="s">
+        <v>67</v>
+      </c>
+      <c r="D77" t="s">
         <v>75</v>
       </c>
-      <c r="E76" s="1">
-        <v>46.800000000000004</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A77" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B77">
-        <v>2023</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E77" s="1">
+      <c r="E77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78">
+        <v>2023</v>
+      </c>
+      <c r="C78" t="s">
+        <v>72</v>
+      </c>
+      <c r="D78" t="s">
+        <v>73</v>
+      </c>
+      <c r="E78">
+        <v>28.999999999999996</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79">
+        <v>2023</v>
+      </c>
+      <c r="C79" t="s">
+        <v>72</v>
+      </c>
+      <c r="D79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>5</v>
+      </c>
+      <c r="B80">
+        <v>2023</v>
+      </c>
+      <c r="C80" t="s">
+        <v>72</v>
+      </c>
+      <c r="D80" t="s">
+        <v>75</v>
+      </c>
+      <c r="E80">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81">
+        <v>2023</v>
+      </c>
+      <c r="C81" t="s">
+        <v>71</v>
+      </c>
+      <c r="D81" t="s">
+        <v>73</v>
+      </c>
+      <c r="E81">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82">
+        <v>2023</v>
+      </c>
+      <c r="C82" t="s">
+        <v>71</v>
+      </c>
+      <c r="D82" t="s">
+        <v>74</v>
+      </c>
+      <c r="E82">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83">
+        <v>2023</v>
+      </c>
+      <c r="C83" t="s">
+        <v>71</v>
+      </c>
+      <c r="D83" t="s">
+        <v>75</v>
+      </c>
+      <c r="E83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84">
+        <v>1961</v>
+      </c>
+      <c r="C84" t="s">
+        <v>18</v>
+      </c>
+      <c r="D84" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84">
+        <v>40000000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85">
+        <v>1961</v>
+      </c>
+      <c r="C85" t="s">
+        <v>48</v>
+      </c>
+      <c r="D85" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E85">
+        <v>11.799999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86">
+        <v>1961</v>
+      </c>
+      <c r="C86" t="s">
+        <v>49</v>
+      </c>
+      <c r="D86" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E86">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87">
+        <v>1961</v>
+      </c>
+      <c r="C87" t="s">
+        <v>50</v>
+      </c>
+      <c r="D87" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E87">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88">
+        <v>1961</v>
+      </c>
+      <c r="C88" t="s">
+        <v>19</v>
+      </c>
+      <c r="D88" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E88">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89">
+        <v>1961</v>
+      </c>
+      <c r="C89" t="s">
+        <v>66</v>
+      </c>
+      <c r="D89" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E89">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90">
+        <v>1961</v>
+      </c>
+      <c r="C90" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A78" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B78">
-        <v>2023</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E78" s="1">
-        <v>28.999999999999996</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B79">
-        <v>2023</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E79" s="1">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A80" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B80">
-        <v>2023</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E80" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A81" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B81">
-        <v>2023</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E81" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A82" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B82">
-        <v>2023</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E82" s="1">
+      <c r="D90" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E90">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91">
+        <v>2023</v>
+      </c>
+      <c r="C91" t="s">
+        <v>18</v>
+      </c>
+      <c r="D91" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E91">
+        <v>70000000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92">
+        <v>2023</v>
+      </c>
+      <c r="C92" t="s">
+        <v>48</v>
+      </c>
+      <c r="D92" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E92">
+        <v>11.799999999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93">
+        <v>2023</v>
+      </c>
+      <c r="C93" t="s">
+        <v>49</v>
+      </c>
+      <c r="D93" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E93">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94">
+        <v>2023</v>
+      </c>
+      <c r="C94" t="s">
+        <v>50</v>
+      </c>
+      <c r="D94" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E94">
         <v>0.2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A83" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B83">
-        <v>2023</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E83" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A84" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B84">
-        <v>1961</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D84" s="5" t="s">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>5</v>
+      </c>
+      <c r="B95">
+        <v>2023</v>
+      </c>
+      <c r="C95" t="s">
+        <v>19</v>
+      </c>
+      <c r="D95" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E84" s="1">
-        <v>40000000</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A85" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B85">
-        <v>1961</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D85" s="6" t="s">
+      <c r="E95">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96">
+        <v>2023</v>
+      </c>
+      <c r="C96" t="s">
+        <v>66</v>
+      </c>
+      <c r="D96" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E85" s="1">
-        <v>11.799999999999999</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A86" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B86">
-        <v>1961</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D86" s="5" t="s">
+      <c r="E96">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97">
+        <v>2023</v>
+      </c>
+      <c r="C97" t="s">
+        <v>20</v>
+      </c>
+      <c r="D97" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E86" s="1">
-        <v>42.5</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A87" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B87">
-        <v>1961</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D87" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E87" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A88" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B88">
-        <v>1961</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E88" s="1">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A89" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B89">
-        <v>1961</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E89" s="1">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A90" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B90">
-        <v>1961</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D90" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E90" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A91" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B91">
-        <v>2023</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E91" s="1">
-        <v>70000000</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A92" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B92">
-        <v>2023</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D92" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E92" s="1">
-        <v>11.799999999999999</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A93" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B93">
-        <v>2023</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D93" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E93" s="1">
-        <v>42.5</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A94" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B94">
-        <v>2023</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D94" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E94" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A95" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B95">
-        <v>2023</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D95" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E95" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A96" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B96">
-        <v>2023</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D96" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E96" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A97" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B97">
-        <v>2023</v>
-      </c>
-      <c r="C97" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E97" s="7">
+      <c r="E97">
         <v>10</v>
       </c>
     </row>
@@ -2497,7 +2525,7 @@
         <v>23</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E99" s="1">
         <v>40</v>
@@ -2616,7 +2644,7 @@
         <v>23</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E106" s="1">
         <v>40</v>
@@ -2735,7 +2763,7 @@
         <v>24</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E113">
         <v>0.03</v>
@@ -2854,7 +2882,7 @@
         <v>24</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E120">
         <v>0.03</v>
@@ -2953,13 +2981,13 @@
         <v>1961</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E126">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
@@ -2970,13 +2998,13 @@
         <v>2023</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E127">
-        <v>150</v>
+        <v>300</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
@@ -2987,13 +3015,13 @@
         <v>1961</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E128">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
@@ -3004,13 +3032,13 @@
         <v>2023</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E129">
-        <v>300</v>
+        <v>70</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
@@ -3021,13 +3049,13 @@
         <v>1961</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E130">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
@@ -3038,13 +3066,13 @@
         <v>2023</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E131">
-        <v>70</v>
+        <v>8</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
@@ -3055,13 +3083,13 @@
         <v>1961</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E132">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
@@ -3069,16 +3097,16 @@
         <v>5</v>
       </c>
       <c r="B133">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E133">
-        <v>8</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
@@ -3086,13 +3114,13 @@
         <v>5</v>
       </c>
       <c r="B134">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E134">
         <v>1</v>
@@ -3103,16 +3131,16 @@
         <v>5</v>
       </c>
       <c r="B135">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E135">
-        <v>10</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
@@ -3123,13 +3151,13 @@
         <v>2023</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E136">
-        <v>1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
@@ -3137,16 +3165,16 @@
         <v>5</v>
       </c>
       <c r="B137">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E137">
-        <v>0.5</v>
+        <v>61</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
@@ -3157,13 +3185,13 @@
         <v>2023</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E138">
-        <v>0.05</v>
+        <v>61</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
@@ -3171,16 +3199,16 @@
         <v>5</v>
       </c>
       <c r="B139">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>63</v>
+        <v>25</v>
+      </c>
+      <c r="D139" t="s">
+        <v>14</v>
+      </c>
+      <c r="E139" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
@@ -3191,13 +3219,13 @@
         <v>2023</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>64</v>
+        <v>25</v>
+      </c>
+      <c r="D140" t="s">
+        <v>15</v>
+      </c>
+      <c r="E140" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
@@ -3208,13 +3236,13 @@
         <v>2023</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D141" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E141" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
@@ -3222,16 +3250,16 @@
         <v>5</v>
       </c>
       <c r="B142">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D142" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E142" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
@@ -3239,16 +3267,16 @@
         <v>5</v>
       </c>
       <c r="B143">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D143" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E143" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
@@ -3259,143 +3287,143 @@
         <v>1961</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D144" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E144" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A145" s="1" t="s">
+      <c r="A145" t="s">
         <v>5</v>
       </c>
       <c r="B145">
         <v>1961</v>
       </c>
-      <c r="C145" s="1" t="s">
-        <v>26</v>
+      <c r="C145" t="s">
+        <v>25</v>
       </c>
       <c r="D145" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="E145" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A146" s="1" t="s">
+      <c r="A146" t="s">
         <v>5</v>
       </c>
       <c r="B146">
-        <v>1961</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>26</v>
+        <v>2023</v>
+      </c>
+      <c r="C146" t="s">
+        <v>25</v>
       </c>
       <c r="D146" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="E146" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A147" s="10" t="s">
+      <c r="A147" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B147" s="2">
         <v>1961</v>
       </c>
       <c r="C147" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D147" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E147" s="8">
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A148" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B148" s="3">
+        <v>1961</v>
+      </c>
+      <c r="C148" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D148" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E148" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A149" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B149" s="2">
+        <v>1961</v>
+      </c>
+      <c r="C149" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="D147" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E147" s="9">
-        <v>2.76</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A148" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B148" s="3">
-        <v>1961</v>
-      </c>
-      <c r="C148" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D148" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E148" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A149" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B149" s="2">
-        <v>1961</v>
-      </c>
-      <c r="C149" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="D149" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E149" s="9">
+      <c r="E149" s="8">
         <v>2.5</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A150" s="11" t="s">
+      <c r="A150" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B150" s="3">
         <v>1961</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E150" s="9">
+        <v>58</v>
+      </c>
+      <c r="E150" s="8">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A151" s="10" t="s">
+      <c r="A151" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B151" s="2">
         <v>1961</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D151" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E151" s="9">
+      <c r="E151" s="8">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A152" s="11" t="s">
+      <c r="A152" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B152" s="3">
         <v>1961</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D152" s="6" t="s">
         <v>8</v>
@@ -3405,116 +3433,116 @@
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A153" s="10" t="s">
+      <c r="A153" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B153" s="2">
         <v>1961</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D153" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E153" s="9">
+      <c r="E153" s="8">
         <v>3.5</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A154" s="11" t="s">
+      <c r="A154" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B154" s="3">
         <v>1961</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D154" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E154" s="12">
+      <c r="E154" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A155" s="10" t="s">
+      <c r="A155" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B155" s="2">
         <v>1961</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D155" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E155" s="13">
+      <c r="E155" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A156" s="10" t="s">
+      <c r="A156" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B156" s="2">
         <v>2023</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D156" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E156" s="9">
+      <c r="E156" s="8">
         <v>2.5</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A157" s="11" t="s">
+      <c r="A157" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B157" s="3">
         <v>2023</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E157" s="9">
+        <v>58</v>
+      </c>
+      <c r="E157" s="8">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A158" s="10" t="s">
+      <c r="A158" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B158" s="2">
         <v>2023</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D158" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E158" s="9">
+      <c r="E158" s="8">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A159" s="11" t="s">
+      <c r="A159" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B159" s="3">
         <v>2023</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D159" s="6" t="s">
         <v>8</v>
@@ -3524,65 +3552,65 @@
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A160" s="10" t="s">
+      <c r="A160" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B160" s="2">
         <v>2023</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D160" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E160" s="9">
+      <c r="E160" s="8">
         <v>3.5</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A161" s="11" t="s">
+      <c r="A161" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B161" s="3">
         <v>2023</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D161" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E161" s="12">
+      <c r="E161" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A162" s="10" t="s">
+      <c r="A162" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B162" s="2">
         <v>2023</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D162" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E162" s="13">
+      <c r="E162" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A163" s="10" t="s">
+      <c r="A163" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B163" s="2">
         <v>1961</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D163" s="5" t="s">
         <v>6</v>
@@ -3592,31 +3620,31 @@
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A164" s="11" t="s">
+      <c r="A164" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B164" s="3">
         <v>1961</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E164">
         <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A165" s="10" t="s">
+      <c r="A165" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B165" s="2">
         <v>1961</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D165" s="5" t="s">
         <v>7</v>
@@ -3626,14 +3654,14 @@
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A166" s="11" t="s">
+      <c r="A166" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B166" s="3">
         <v>1961</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D166" s="6" t="s">
         <v>8</v>
@@ -3643,14 +3671,14 @@
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A167" s="10" t="s">
+      <c r="A167" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B167" s="2">
         <v>1961</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D167" s="5" t="s">
         <v>9</v>
@@ -3660,14 +3688,14 @@
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A168" s="11" t="s">
+      <c r="A168" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B168" s="3">
         <v>1961</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D168" s="6" t="s">
         <v>11</v>
@@ -3677,14 +3705,14 @@
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A169" s="10" t="s">
+      <c r="A169" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B169" s="2">
         <v>1961</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D169" s="5" t="s">
         <v>22</v>
@@ -3694,14 +3722,14 @@
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A170" s="10" t="s">
+      <c r="A170" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B170" s="2">
         <v>2023</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D170" s="5" t="s">
         <v>6</v>
@@ -3711,31 +3739,31 @@
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A171" s="11" t="s">
+      <c r="A171" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B171" s="3">
         <v>2023</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E171">
         <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A172" s="10" t="s">
+      <c r="A172" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B172" s="2">
         <v>2023</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D172" s="5" t="s">
         <v>7</v>
@@ -3745,14 +3773,14 @@
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A173" s="11" t="s">
+      <c r="A173" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B173" s="3">
         <v>2023</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D173" s="6" t="s">
         <v>8</v>
@@ -3762,14 +3790,14 @@
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A174" s="10" t="s">
+      <c r="A174" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B174" s="2">
         <v>2023</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D174" s="5" t="s">
         <v>9</v>
@@ -3779,14 +3807,14 @@
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A175" s="11" t="s">
+      <c r="A175" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B175" s="3">
         <v>2023</v>
       </c>
       <c r="C175" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D175" s="6" t="s">
         <v>11</v>
@@ -3796,14 +3824,14 @@
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A176" s="10" t="s">
+      <c r="A176" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B176" s="2">
         <v>2023</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D176" s="5" t="s">
         <v>22</v>
@@ -3813,34 +3841,34 @@
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A177" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B177" s="15">
-        <v>1961</v>
-      </c>
-      <c r="C177" s="16" t="s">
+      <c r="A177" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B177" s="14">
+        <v>1961</v>
+      </c>
+      <c r="C177" s="15" t="s">
         <v>12</v>
       </c>
       <c r="D177" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E177">
         <v>20</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A178" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B178" s="15">
-        <v>2023</v>
-      </c>
-      <c r="C178" s="16" t="s">
+      <c r="A178" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B178" s="14">
+        <v>2023</v>
+      </c>
+      <c r="C178" s="15" t="s">
         <v>12</v>
       </c>
       <c r="D178" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E178">
         <v>25</v>
@@ -3857,10 +3885,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80ABBC0-87F2-4F7A-9036-33771C52D9AC}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3869,316 +3897,316 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>0.65</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>0.1</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>0.25</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>0.3</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>0.1</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>0.2</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>0.4</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>0.6</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10">
         <v>0.1</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>0.05</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>0.1</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>0.05</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14">
         <v>0.1</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15">
         <v>0.5</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18">
         <v>0.3</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19">
         <v>0.1</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>0.2</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21">
         <v>0.4</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22">
         <v>0.3</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23">
         <v>0.05</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25">
         <v>0.05</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27">
         <v>0.05</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28">
         <v>0.3</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29">
         <v>0.05</v>
@@ -4189,13 +4217,57 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30">
         <v>0.15</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31">
+        <v>0.2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32">
+        <v>0.1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33">
+        <v>0.6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34">
+        <v>0.1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correction des fichiers exemple de C (seed + fish)
</commit_message>
<xml_diff>
--- a/example/GRAFS_data_example_C.xlsx
+++ b/example/GRAFS_data_example_C.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faustega\Documents\These\isterre-dynamic-modeling\grafs-e-project\grafs-e\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E999C94C-9619-4381-B2C7-6308807B731E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F03168-A32D-4F40-AACD-8FEEB55A0239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16530" yWindow="-15870" windowWidth="25440" windowHeight="15270" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
   </bookViews>
   <sheets>
     <sheet name="Input data" sheetId="2" r:id="rId1"/>
     <sheet name="Diet" sheetId="3" r:id="rId2"/>
+    <sheet name="Energy power" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="DonnéesExternes_1" localSheetId="0" hidden="1">'Input data'!$A$1:$E$97</definedName>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="89">
   <si>
     <t>Area</t>
   </si>
@@ -251,9 +252,6 @@
     <t>Meat of pig with the bone fresh or chilled</t>
   </si>
   <si>
-    <t>Fischery ingestion per capita (kgN)</t>
-  </si>
-  <si>
     <t>N-NH3 EM (%)</t>
   </si>
   <si>
@@ -297,6 +295,30 @@
   </si>
   <si>
     <t>Methanizer</t>
+  </si>
+  <si>
+    <t>Fishery ingestion per capita (kgN)</t>
+  </si>
+  <si>
+    <t>Bio_diet</t>
+  </si>
+  <si>
+    <t>Forage</t>
+  </si>
+  <si>
+    <t>Facility</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>Bioraffinery</t>
+  </si>
+  <si>
+    <t>Energy Power (MWh/tFW)</t>
+  </si>
+  <si>
+    <t>Wheat grain, Oats grain</t>
   </si>
 </sst>
 </file>
@@ -442,6 +464,9 @@
   <dxfs count="4">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -454,9 +479,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -508,8 +530,8 @@
     <tableColumn id="3" xr3:uid="{7B352F64-988D-49A0-B664-7D1BD688EE1B}" uniqueName="3" name="Area" queryTableFieldId="3" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{E88EBC76-2C3C-4BE6-B345-902903CB70D2}" uniqueName="4" name="Year" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{C56568E9-7386-48BB-AE51-0A3400CB0D14}" uniqueName="5" name="category" queryTableFieldId="5" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{583513EB-334C-4C54-BF53-D669A066B6B7}" uniqueName="10" name="item" queryTableFieldId="10" dataDxfId="0"/>
-    <tableColumn id="11" xr3:uid="{91174CF9-2FC0-4CE8-B60F-7E15C76A8221}" uniqueName="11" name="value" queryTableFieldId="11" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{583513EB-334C-4C54-BF53-D669A066B6B7}" uniqueName="10" name="item" queryTableFieldId="10" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{91174CF9-2FC0-4CE8-B60F-7E15C76A8221}" uniqueName="11" name="value" queryTableFieldId="11" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -832,11 +854,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D825A9-0C1C-44E4-98B7-F194F26ABDB6}">
-  <dimension ref="A1:E178"/>
+  <dimension ref="A1:E176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E55" sqref="E55"/>
+      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A132" sqref="A132:XFD132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1519,10 +1541,10 @@
         <v>1961</v>
       </c>
       <c r="C40" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" t="s">
         <v>67</v>
-      </c>
-      <c r="D40" t="s">
-        <v>68</v>
       </c>
       <c r="E40">
         <v>46.800000000000004</v>
@@ -1536,10 +1558,10 @@
         <v>1961</v>
       </c>
       <c r="C41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E41">
         <v>10</v>
@@ -1553,10 +1575,10 @@
         <v>1961</v>
       </c>
       <c r="C42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E42">
         <v>40</v>
@@ -1570,10 +1592,10 @@
         <v>1961</v>
       </c>
       <c r="C43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E43">
         <v>30</v>
@@ -1587,10 +1609,10 @@
         <v>1961</v>
       </c>
       <c r="C44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E44">
         <v>15</v>
@@ -1604,10 +1626,10 @@
         <v>1961</v>
       </c>
       <c r="C45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E45">
         <v>0.5</v>
@@ -1621,10 +1643,10 @@
         <v>1961</v>
       </c>
       <c r="C46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E46">
         <v>0.25</v>
@@ -1638,10 +1660,10 @@
         <v>1961</v>
       </c>
       <c r="C47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E47">
         <v>2</v>
@@ -1706,10 +1728,10 @@
         <v>1961</v>
       </c>
       <c r="C51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E51">
         <v>35.880000000000003</v>
@@ -1723,10 +1745,10 @@
         <v>1961</v>
       </c>
       <c r="C52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E52">
         <v>46.800000000000004</v>
@@ -1740,10 +1762,10 @@
         <v>1961</v>
       </c>
       <c r="C53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D53" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E53">
         <v>10</v>
@@ -1757,10 +1779,10 @@
         <v>1961</v>
       </c>
       <c r="C54" t="s">
+        <v>71</v>
+      </c>
+      <c r="D54" t="s">
         <v>72</v>
-      </c>
-      <c r="D54" t="s">
-        <v>73</v>
       </c>
       <c r="E54">
         <v>35</v>
@@ -1774,10 +1796,10 @@
         <v>1961</v>
       </c>
       <c r="C55" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E55">
         <v>25</v>
@@ -1791,10 +1813,10 @@
         <v>1961</v>
       </c>
       <c r="C56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D56" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E56">
         <v>30</v>
@@ -1808,10 +1830,10 @@
         <v>1961</v>
       </c>
       <c r="C57" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E57">
         <v>4</v>
@@ -1825,10 +1847,10 @@
         <v>1961</v>
       </c>
       <c r="C58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E58">
         <v>0.2</v>
@@ -1842,10 +1864,10 @@
         <v>1961</v>
       </c>
       <c r="C59" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D59" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E59">
         <v>2</v>
@@ -1910,10 +1932,10 @@
         <v>2023</v>
       </c>
       <c r="C63" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D63" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E63">
         <v>35.880000000000003</v>
@@ -1927,10 +1949,10 @@
         <v>2023</v>
       </c>
       <c r="C64" t="s">
+        <v>66</v>
+      </c>
+      <c r="D64" t="s">
         <v>67</v>
-      </c>
-      <c r="D64" t="s">
-        <v>68</v>
       </c>
       <c r="E64">
         <v>46.800000000000004</v>
@@ -1944,10 +1966,10 @@
         <v>2023</v>
       </c>
       <c r="C65" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E65">
         <v>10</v>
@@ -1961,10 +1983,10 @@
         <v>2023</v>
       </c>
       <c r="C66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E66">
         <v>2.5</v>
@@ -1978,10 +2000,10 @@
         <v>2023</v>
       </c>
       <c r="C67" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E67">
         <v>1.25</v>
@@ -1995,10 +2017,10 @@
         <v>2023</v>
       </c>
       <c r="C68" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E68">
         <v>10</v>
@@ -2012,10 +2034,10 @@
         <v>2023</v>
       </c>
       <c r="C69" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E69">
         <v>0.5</v>
@@ -2029,10 +2051,10 @@
         <v>2023</v>
       </c>
       <c r="C70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D70" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E70">
         <v>0.25</v>
@@ -2046,10 +2068,10 @@
         <v>2023</v>
       </c>
       <c r="C71" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E71">
         <v>2</v>
@@ -2114,10 +2136,10 @@
         <v>2023</v>
       </c>
       <c r="C75" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E75">
         <v>35.880000000000003</v>
@@ -2131,10 +2153,10 @@
         <v>2023</v>
       </c>
       <c r="C76" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E76">
         <v>46.800000000000004</v>
@@ -2148,10 +2170,10 @@
         <v>2023</v>
       </c>
       <c r="C77" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D77" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E77">
         <v>10</v>
@@ -2165,10 +2187,10 @@
         <v>2023</v>
       </c>
       <c r="C78" t="s">
+        <v>71</v>
+      </c>
+      <c r="D78" t="s">
         <v>72</v>
-      </c>
-      <c r="D78" t="s">
-        <v>73</v>
       </c>
       <c r="E78">
         <v>28.999999999999996</v>
@@ -2182,10 +2204,10 @@
         <v>2023</v>
       </c>
       <c r="C79" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D79" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -2199,10 +2221,10 @@
         <v>2023</v>
       </c>
       <c r="C80" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D80" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E80">
         <v>10</v>
@@ -2216,10 +2238,10 @@
         <v>2023</v>
       </c>
       <c r="C81" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E81">
         <v>4</v>
@@ -2233,10 +2255,10 @@
         <v>2023</v>
       </c>
       <c r="C82" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D82" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E82">
         <v>0.2</v>
@@ -2250,10 +2272,10 @@
         <v>2023</v>
       </c>
       <c r="C83" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D83" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E83">
         <v>2</v>
@@ -2352,7 +2374,7 @@
         <v>1961</v>
       </c>
       <c r="C89" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="D89" s="17" t="s">
         <v>21</v>
@@ -2471,7 +2493,7 @@
         <v>2023</v>
       </c>
       <c r="C96" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="D96" s="17" t="s">
         <v>21</v>
@@ -3080,7 +3102,7 @@
         <v>5</v>
       </c>
       <c r="B132">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>35</v>
@@ -3097,7 +3119,7 @@
         <v>5</v>
       </c>
       <c r="B133">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>35</v>
@@ -3120,10 +3142,10 @@
         <v>35</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E134">
-        <v>1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
@@ -3131,16 +3153,16 @@
         <v>5</v>
       </c>
       <c r="B135">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E135">
-        <v>0.5</v>
+        <v>61</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
@@ -3154,10 +3176,10 @@
         <v>35</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E136">
-        <v>0.05</v>
+        <v>61</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
@@ -3165,16 +3187,16 @@
         <v>5</v>
       </c>
       <c r="B137">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>62</v>
+        <v>25</v>
+      </c>
+      <c r="D137" t="s">
+        <v>14</v>
+      </c>
+      <c r="E137" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
@@ -3185,13 +3207,13 @@
         <v>2023</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>63</v>
+        <v>25</v>
+      </c>
+      <c r="D138" t="s">
+        <v>15</v>
+      </c>
+      <c r="E138" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
@@ -3205,10 +3227,10 @@
         <v>25</v>
       </c>
       <c r="D139" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E139" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
@@ -3216,16 +3238,16 @@
         <v>5</v>
       </c>
       <c r="B140">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D140" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E140" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
@@ -3233,16 +3255,16 @@
         <v>5</v>
       </c>
       <c r="B141">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D141" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E141" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
@@ -3256,78 +3278,78 @@
         <v>25</v>
       </c>
       <c r="D142" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E142" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A143" s="1" t="s">
+      <c r="A143" t="s">
         <v>5</v>
       </c>
       <c r="B143">
         <v>1961</v>
       </c>
-      <c r="C143" s="1" t="s">
+      <c r="C143" t="s">
         <v>25</v>
       </c>
       <c r="D143" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="E143" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A144" s="1" t="s">
+      <c r="A144" t="s">
         <v>5</v>
       </c>
       <c r="B144">
-        <v>1961</v>
-      </c>
-      <c r="C144" s="1" t="s">
+        <v>2023</v>
+      </c>
+      <c r="C144" t="s">
         <v>25</v>
       </c>
       <c r="D144" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="E144" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A145" t="s">
-        <v>5</v>
-      </c>
-      <c r="B145">
-        <v>1961</v>
-      </c>
-      <c r="C145" t="s">
-        <v>25</v>
-      </c>
-      <c r="D145" t="s">
-        <v>81</v>
-      </c>
-      <c r="E145" t="s">
-        <v>77</v>
+      <c r="A145" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B145" s="2">
+        <v>1961</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D145" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E145" s="8">
+        <v>2.76</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A146" t="s">
-        <v>5</v>
-      </c>
-      <c r="B146">
-        <v>2023</v>
-      </c>
-      <c r="C146" t="s">
-        <v>25</v>
-      </c>
-      <c r="D146" t="s">
-        <v>81</v>
-      </c>
-      <c r="E146" t="s">
-        <v>77</v>
+      <c r="A146" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B146" s="3">
+        <v>1961</v>
+      </c>
+      <c r="C146" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D146" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E146" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
@@ -3338,13 +3360,13 @@
         <v>1961</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="E147" s="8">
-        <v>2.76</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
@@ -3354,14 +3376,14 @@
       <c r="B148" s="3">
         <v>1961</v>
       </c>
-      <c r="C148" s="6" t="s">
-        <v>32</v>
+      <c r="C148" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E148" s="8">
-        <v>1</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
@@ -3375,10 +3397,10 @@
         <v>33</v>
       </c>
       <c r="D149" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E149" s="8">
-        <v>2.5</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
@@ -3392,10 +3414,10 @@
         <v>33</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E150" s="8">
-        <v>2.2000000000000002</v>
+        <v>8</v>
+      </c>
+      <c r="E150" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
@@ -3409,10 +3431,10 @@
         <v>33</v>
       </c>
       <c r="D151" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E151" s="8">
-        <v>2.2000000000000002</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.35">
@@ -3426,9 +3448,9 @@
         <v>33</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E152" s="4">
+        <v>11</v>
+      </c>
+      <c r="E152" s="11">
         <v>0</v>
       </c>
     </row>
@@ -3443,44 +3465,44 @@
         <v>33</v>
       </c>
       <c r="D153" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E153" s="8">
-        <v>3.5</v>
+        <v>22</v>
+      </c>
+      <c r="E153" s="12">
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A154" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B154" s="3">
-        <v>1961</v>
+      <c r="A154" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B154" s="2">
+        <v>2023</v>
       </c>
       <c r="C154" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D154" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E154" s="11">
-        <v>0</v>
+      <c r="D154" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E154" s="8">
+        <v>2.5</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A155" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B155" s="2">
-        <v>1961</v>
+      <c r="A155" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B155" s="3">
+        <v>2023</v>
       </c>
       <c r="C155" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D155" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E155" s="12">
-        <v>0</v>
+      <c r="D155" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E155" s="8">
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
@@ -3494,10 +3516,10 @@
         <v>33</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E156" s="8">
-        <v>2.5</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
@@ -3511,10 +3533,10 @@
         <v>33</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E157" s="8">
-        <v>2.2000000000000002</v>
+        <v>8</v>
+      </c>
+      <c r="E157" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
@@ -3528,10 +3550,10 @@
         <v>33</v>
       </c>
       <c r="D158" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E158" s="8">
-        <v>2.2000000000000002</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
@@ -3545,9 +3567,9 @@
         <v>33</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E159" s="4">
+        <v>11</v>
+      </c>
+      <c r="E159" s="11">
         <v>0</v>
       </c>
     </row>
@@ -3562,43 +3584,43 @@
         <v>33</v>
       </c>
       <c r="D160" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E160" s="8">
-        <v>3.5</v>
+        <v>22</v>
+      </c>
+      <c r="E160" s="12">
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A161" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B161" s="3">
-        <v>2023</v>
+      <c r="A161" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B161" s="2">
+        <v>1961</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D161" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E161" s="11">
+        <v>34</v>
+      </c>
+      <c r="D161" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E161">
         <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A162" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B162" s="2">
-        <v>2023</v>
+      <c r="A162" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B162" s="3">
+        <v>1961</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D162" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E162" s="12">
+        <v>34</v>
+      </c>
+      <c r="D162" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E162">
         <v>0</v>
       </c>
     </row>
@@ -3613,7 +3635,7 @@
         <v>34</v>
       </c>
       <c r="D163" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E163">
         <v>0</v>
@@ -3630,10 +3652,10 @@
         <v>34</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="E164">
-        <v>0</v>
+        <v>125</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.35">
@@ -3647,7 +3669,7 @@
         <v>34</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E165">
         <v>0</v>
@@ -3664,10 +3686,10 @@
         <v>34</v>
       </c>
       <c r="D166" s="6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E166">
-        <v>125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.35">
@@ -3681,44 +3703,44 @@
         <v>34</v>
       </c>
       <c r="D167" s="5" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E167">
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A168" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B168" s="3">
-        <v>1961</v>
+      <c r="A168" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B168" s="2">
+        <v>2023</v>
       </c>
       <c r="C168" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D168" s="6" t="s">
-        <v>11</v>
+      <c r="D168" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="E168">
         <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A169" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B169" s="2">
-        <v>1961</v>
+      <c r="A169" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B169" s="3">
+        <v>2023</v>
       </c>
       <c r="C169" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D169" s="5" t="s">
-        <v>22</v>
+      <c r="D169" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="E169">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.35">
@@ -3732,7 +3754,7 @@
         <v>34</v>
       </c>
       <c r="D170" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E170">
         <v>0</v>
@@ -3749,10 +3771,10 @@
         <v>34</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="E171">
-        <v>0</v>
+        <v>125</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.35">
@@ -3766,7 +3788,7 @@
         <v>34</v>
       </c>
       <c r="D172" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E172">
         <v>0</v>
@@ -3783,10 +3805,10 @@
         <v>34</v>
       </c>
       <c r="D173" s="6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E173">
-        <v>125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.35">
@@ -3800,77 +3822,43 @@
         <v>34</v>
       </c>
       <c r="D174" s="5" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E174">
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A175" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B175" s="3">
-        <v>2023</v>
-      </c>
-      <c r="C175" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D175" s="6" t="s">
-        <v>11</v>
+      <c r="A175" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B175" s="14">
+        <v>1961</v>
+      </c>
+      <c r="C175" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D175" t="s">
+        <v>39</v>
       </c>
       <c r="E175">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A176" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B176" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C176" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D176" s="5" t="s">
-        <v>22</v>
+      <c r="A176" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B176" s="14">
+        <v>2023</v>
+      </c>
+      <c r="C176" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D176" t="s">
+        <v>39</v>
       </c>
       <c r="E176">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A177" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B177" s="14">
-        <v>1961</v>
-      </c>
-      <c r="C177" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D177" t="s">
-        <v>39</v>
-      </c>
-      <c r="E177">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A178" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B178" s="14">
-        <v>2023</v>
-      </c>
-      <c r="C178" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D178" t="s">
-        <v>39</v>
-      </c>
-      <c r="E178">
         <v>25</v>
       </c>
     </row>
@@ -3885,14 +3873,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80ABBC0-87F2-4F7A-9036-33771C52D9AC}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="20.90625" customWidth="1"/>
     <col min="3" max="3" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3915,7 +3904,7 @@
         <v>0.65</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -4058,7 +4047,7 @@
         <v>0.5</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -4228,46 +4217,164 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31">
         <v>0.2</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B32">
         <v>0.1</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B33">
         <v>0.6</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B34">
         <v>0.1</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35">
+        <v>0.5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36">
+        <v>0.5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A837CEBA-F317-4ADF-A0E2-18BECAC8E8AA}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="26.90625" customWidth="1"/>
+    <col min="3" max="3" width="21.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Des progrès. Mise en place des mécanismes pour le mode prospective. Il faut...
</commit_message>
<xml_diff>
--- a/example/GRAFS_data_example_C.xlsx
+++ b/example/GRAFS_data_example_C.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faustega\Documents\These\isterre-dynamic-modeling\grafs-e-project\grafs-e\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F03168-A32D-4F40-AACD-8FEEB55A0239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429E9E6A-F458-401A-8273-C4C3197E2FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
+    <workbookView xWindow="-12270" yWindow="-16350" windowWidth="29040" windowHeight="15720" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
   </bookViews>
   <sheets>
     <sheet name="Input data" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Energy power" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="DonnéesExternes_1" localSheetId="0" hidden="1">'Input data'!$A$1:$E$97</definedName>
+    <definedName name="DonnéesExternes_1" localSheetId="0" hidden="1">'Input data'!$A$1:$E$175</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="89">
   <si>
     <t>Area</t>
   </si>
@@ -90,235 +90,235 @@
     <t>Soya beans</t>
   </si>
   <si>
+    <t>Area (ha)</t>
+  </si>
+  <si>
+    <t>bovines</t>
+  </si>
+  <si>
+    <t>porcines</t>
+  </si>
+  <si>
+    <t>Excretion / LU (kgN)</t>
+  </si>
+  <si>
+    <t>LU</t>
+  </si>
+  <si>
+    <t>Inhabitants</t>
+  </si>
+  <si>
+    <t>Total ingestion per capita (kgN)</t>
+  </si>
+  <si>
+    <t>Excretion recycling (%)</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Natural meadow</t>
+  </si>
+  <si>
+    <t>Spreading Rate (%)</t>
+  </si>
+  <si>
+    <t>Seed input (kt seeds/kt Ymax)</t>
+  </si>
+  <si>
+    <t>Diet</t>
+  </si>
+  <si>
+    <t>b_2023_fr</t>
+  </si>
+  <si>
+    <t>p_2023_fr</t>
+  </si>
+  <si>
+    <t>fr_2023_fr</t>
+  </si>
+  <si>
+    <t>Proportion</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>Diet ID</t>
+  </si>
+  <si>
+    <t>Nitrogen Content (%)</t>
+  </si>
+  <si>
+    <t>Fertilization Need (kgN/qtl)</t>
+  </si>
+  <si>
+    <t>Surface Fertilization Need (kgN/ha)</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>b_1961_fr</t>
+  </si>
+  <si>
+    <t>p_1961_fr</t>
+  </si>
+  <si>
+    <t>fr_1961_fr</t>
+  </si>
+  <si>
+    <t>Atmospheric deposition coef (kgN/ha)</t>
+  </si>
+  <si>
+    <t>Total Synthetic Fertilizer Use on crops (ktN)</t>
+  </si>
+  <si>
+    <t>Total Synthetic Fertilizer Use on grasslands (ktN)</t>
+  </si>
+  <si>
+    <t>Weight diet</t>
+  </si>
+  <si>
+    <t>Weight import</t>
+  </si>
+  <si>
+    <t>Weight distribution</t>
+  </si>
+  <si>
+    <t>Excreted indoor (%)</t>
+  </si>
+  <si>
+    <t>Excreted indoor as manure (%)</t>
+  </si>
+  <si>
+    <t>N-NH3 EM excretion (%)</t>
+  </si>
+  <si>
+    <t>N-N2 EM excretion (%)</t>
+  </si>
+  <si>
+    <t>N-N2O EM excretion (%)</t>
+  </si>
+  <si>
+    <t>Barley grain</t>
+  </si>
+  <si>
+    <t>Maize corn</t>
+  </si>
+  <si>
+    <t>Oats grain</t>
+  </si>
+  <si>
+    <t>Rice grain</t>
+  </si>
+  <si>
+    <t>Wheat grain</t>
+  </si>
+  <si>
+    <t>Soya beans grain</t>
+  </si>
+  <si>
+    <t>Maize</t>
+  </si>
+  <si>
+    <t>Barley  grain</t>
+  </si>
+  <si>
+    <t>Barley grain, Wheat grain</t>
+  </si>
+  <si>
+    <t>Enforce animal share</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Meat of cattle with the bone fresh or chilled</t>
+  </si>
+  <si>
+    <t>Meat of pig with the bone fresh or chilled</t>
+  </si>
+  <si>
+    <t>N-NH3 EM (%)</t>
+  </si>
+  <si>
+    <t>bovines slurry</t>
+  </si>
+  <si>
+    <t>bovines grasslands excretion</t>
+  </si>
+  <si>
+    <t>bovines manure</t>
+  </si>
+  <si>
+    <t>N-N2O EM (%)</t>
+  </si>
+  <si>
+    <t>N-N2 EM (%)</t>
+  </si>
+  <si>
+    <t>porcines manure</t>
+  </si>
+  <si>
+    <t>porcines slurry</t>
+  </si>
+  <si>
+    <t>porcines grasslands excretion</t>
+  </si>
+  <si>
+    <t>Natural meadow forage, Forage</t>
+  </si>
+  <si>
+    <t>Methanizer_diet</t>
+  </si>
+  <si>
+    <t>bovines slurry, bovines manure, porcines slurry, porcines manure</t>
+  </si>
+  <si>
+    <t>waste</t>
+  </si>
+  <si>
+    <t>Barley grain, Wheat grain, Oats grain, Maize corn</t>
+  </si>
+  <si>
+    <t>Methanizer</t>
+  </si>
+  <si>
+    <t>Fishery ingestion per capita (kgN)</t>
+  </si>
+  <si>
+    <t>Bio_diet</t>
+  </si>
+  <si>
+    <t>Forage</t>
+  </si>
+  <si>
+    <t>Facility</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>Bioraffinery</t>
+  </si>
+  <si>
+    <t>Energy Power (MWh/tFW)</t>
+  </si>
+  <si>
+    <t>Wheat grain, Oats grain</t>
+  </si>
+  <si>
     <t>Production (kton)</t>
   </si>
   <si>
-    <t>Area (ha)</t>
-  </si>
-  <si>
-    <t>bovines</t>
-  </si>
-  <si>
-    <t>porcines</t>
-  </si>
-  <si>
-    <t>Excretion / LU (kgN)</t>
-  </si>
-  <si>
-    <t>LU</t>
-  </si>
-  <si>
-    <t>Inhabitants</t>
-  </si>
-  <si>
-    <t>Total ingestion per capita (kgN)</t>
-  </si>
-  <si>
-    <t>Excretion recycling (%)</t>
-  </si>
-  <si>
-    <t>French</t>
-  </si>
-  <si>
-    <t>Natural meadow</t>
-  </si>
-  <si>
-    <t>Spreading Rate (%)</t>
-  </si>
-  <si>
-    <t>Seed input (kt seeds/kt Ymax)</t>
-  </si>
-  <si>
-    <t>Diet</t>
-  </si>
-  <si>
-    <t>b_2023_fr</t>
-  </si>
-  <si>
-    <t>p_2023_fr</t>
-  </si>
-  <si>
-    <t>fr_2023_fr</t>
-  </si>
-  <si>
-    <t>Proportion</t>
-  </si>
-  <si>
-    <t>Products</t>
-  </si>
-  <si>
-    <t>Diet ID</t>
-  </si>
-  <si>
-    <t>Nitrogen Content (%)</t>
-  </si>
-  <si>
-    <t>Fertilization Need (kgN/qtl)</t>
-  </si>
-  <si>
-    <t>Surface Fertilization Need (kgN/ha)</t>
-  </si>
-  <si>
-    <t>Global</t>
-  </si>
-  <si>
-    <t>b_1961_fr</t>
-  </si>
-  <si>
-    <t>p_1961_fr</t>
-  </si>
-  <si>
-    <t>fr_1961_fr</t>
+    <t>Natural meadow forage</t>
   </si>
   <si>
     <t>Non edible porcines carcass</t>
-  </si>
-  <si>
-    <t>Atmospheric deposition coef (kgN/ha)</t>
-  </si>
-  <si>
-    <t>Total Synthetic Fertilizer Use on crops (ktN)</t>
-  </si>
-  <si>
-    <t>Total Synthetic Fertilizer Use on grasslands (ktN)</t>
-  </si>
-  <si>
-    <t>Weight diet</t>
-  </si>
-  <si>
-    <t>Weight import</t>
-  </si>
-  <si>
-    <t>Weight distribution</t>
-  </si>
-  <si>
-    <t>Excreted indoor (%)</t>
-  </si>
-  <si>
-    <t>Excreted indoor as manure (%)</t>
-  </si>
-  <si>
-    <t>N-NH3 EM excretion (%)</t>
-  </si>
-  <si>
-    <t>N-N2 EM excretion (%)</t>
-  </si>
-  <si>
-    <t>N-N2O EM excretion (%)</t>
-  </si>
-  <si>
-    <t>Barley grain</t>
-  </si>
-  <si>
-    <t>Maize corn</t>
-  </si>
-  <si>
-    <t>Oats grain</t>
-  </si>
-  <si>
-    <t>Rice grain</t>
-  </si>
-  <si>
-    <t>Wheat grain</t>
-  </si>
-  <si>
-    <t>Soya beans grain</t>
-  </si>
-  <si>
-    <t>Natural meadow forage</t>
-  </si>
-  <si>
-    <t>Maize</t>
-  </si>
-  <si>
-    <t>Barley  grain</t>
-  </si>
-  <si>
-    <t>Barley grain, Wheat grain</t>
-  </si>
-  <si>
-    <t>Enforce animal share</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>False</t>
-  </si>
-  <si>
-    <t>Meat of cattle with the bone fresh or chilled</t>
-  </si>
-  <si>
-    <t>Meat of pig with the bone fresh or chilled</t>
-  </si>
-  <si>
-    <t>N-NH3 EM (%)</t>
-  </si>
-  <si>
-    <t>bovines slurry</t>
-  </si>
-  <si>
-    <t>bovines grasslands excretion</t>
-  </si>
-  <si>
-    <t>bovines manure</t>
-  </si>
-  <si>
-    <t>N-N2O EM (%)</t>
-  </si>
-  <si>
-    <t>N-N2 EM (%)</t>
-  </si>
-  <si>
-    <t>porcines manure</t>
-  </si>
-  <si>
-    <t>porcines slurry</t>
-  </si>
-  <si>
-    <t>porcines grasslands excretion</t>
-  </si>
-  <si>
-    <t>Natural meadow forage, Forage</t>
-  </si>
-  <si>
-    <t>Methanizer_diet</t>
-  </si>
-  <si>
-    <t>bovines slurry, bovines manure, porcines slurry, porcines manure</t>
-  </si>
-  <si>
-    <t>waste</t>
-  </si>
-  <si>
-    <t>Barley grain, Wheat grain, Oats grain, Maize corn</t>
-  </si>
-  <si>
-    <t>Methanizer</t>
-  </si>
-  <si>
-    <t>Fishery ingestion per capita (kgN)</t>
-  </si>
-  <si>
-    <t>Bio_diet</t>
-  </si>
-  <si>
-    <t>Forage</t>
-  </si>
-  <si>
-    <t>Facility</t>
-  </si>
-  <si>
-    <t>Items</t>
-  </si>
-  <si>
-    <t>Bioraffinery</t>
-  </si>
-  <si>
-    <t>Energy Power (MWh/tFW)</t>
-  </si>
-  <si>
-    <t>Wheat grain, Oats grain</t>
   </si>
 </sst>
 </file>
@@ -361,7 +361,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -430,11 +430,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -457,6 +466,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,7 +483,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
@@ -476,8 +492,6 @@
         <bottom style="thin">
           <color theme="9" tint="0.39997558519241921"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -524,8 +538,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C19122AA-E7CC-4368-B59D-7B0737AF5C9D}" name="production_france" displayName="production_france" ref="A1:E97" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E97" xr:uid="{C19122AA-E7CC-4368-B59D-7B0737AF5C9D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C19122AA-E7CC-4368-B59D-7B0737AF5C9D}" name="production_france" displayName="production_france" ref="A1:E175" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:E175" xr:uid="{C19122AA-E7CC-4368-B59D-7B0737AF5C9D}"/>
   <tableColumns count="5">
     <tableColumn id="3" xr3:uid="{7B352F64-988D-49A0-B664-7D1BD688EE1B}" uniqueName="3" name="Area" queryTableFieldId="3" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{E88EBC76-2C3C-4BE6-B345-902903CB70D2}" uniqueName="4" name="Year" queryTableFieldId="4"/>
@@ -854,11 +868,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D825A9-0C1C-44E4-98B7-F194F26ABDB6}">
-  <dimension ref="A1:E176"/>
+  <dimension ref="A1:E353"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A132" sqref="A132:XFD132"/>
+      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D168" sqref="D168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -895,10 +909,10 @@
         <v>1961</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E2">
         <v>15000</v>
@@ -912,10 +926,10 @@
         <v>1961</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E3">
         <v>7500</v>
@@ -929,10 +943,10 @@
         <v>1961</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4">
         <v>2590.69</v>
@@ -946,10 +960,10 @@
         <v>1961</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E5">
         <v>133.69</v>
@@ -963,10 +977,10 @@
         <v>1961</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E6">
         <v>25000</v>
@@ -980,10 +994,10 @@
         <v>1961</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E7">
         <v>600</v>
@@ -997,10 +1011,10 @@
         <v>1961</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="E8">
         <v>10000</v>
@@ -1014,10 +1028,10 @@
         <v>1961</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E9">
         <v>1448</v>
@@ -1031,10 +1045,10 @@
         <v>1961</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E10">
         <v>1188</v>
@@ -1048,7 +1062,7 @@
         <v>1961</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -1065,10 +1079,10 @@
         <v>2023</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E12">
         <v>12143.49</v>
@@ -1082,10 +1096,10 @@
         <v>2023</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E13">
         <v>12834.6</v>
@@ -1099,10 +1113,10 @@
         <v>2023</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E14">
         <v>337.34</v>
@@ -1116,10 +1130,10 @@
         <v>2023</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E15">
         <v>68.27</v>
@@ -1133,10 +1147,10 @@
         <v>2023</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E16">
         <v>35995.57</v>
@@ -1150,10 +1164,10 @@
         <v>2023</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E17">
         <v>387.8</v>
@@ -1167,10 +1181,10 @@
         <v>2023</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="E18">
         <v>5000</v>
@@ -1184,10 +1198,10 @@
         <v>2023</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E19">
         <v>1301.42</v>
@@ -1201,10 +1215,10 @@
         <v>2023</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E20">
         <v>2062.46</v>
@@ -1218,7 +1232,7 @@
         <v>2023</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
@@ -1235,7 +1249,7 @@
         <v>1961</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
@@ -1252,10 +1266,10 @@
         <v>1961</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E23">
         <v>980600</v>
@@ -1269,7 +1283,7 @@
         <v>1961</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
@@ -1286,7 +1300,7 @@
         <v>1961</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D25" t="s">
         <v>8</v>
@@ -1303,7 +1317,7 @@
         <v>1961</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D26" t="s">
         <v>9</v>
@@ -1320,7 +1334,7 @@
         <v>1961</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -1337,10 +1351,10 @@
         <v>1961</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E28">
         <v>10000000</v>
@@ -1354,7 +1368,7 @@
         <v>2023</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
@@ -1371,10 +1385,10 @@
         <v>2023</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E30">
         <v>1314680</v>
@@ -1388,7 +1402,7 @@
         <v>2023</v>
       </c>
       <c r="C31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
@@ -1405,7 +1419,7 @@
         <v>2023</v>
       </c>
       <c r="C32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D32" t="s">
         <v>8</v>
@@ -1422,7 +1436,7 @@
         <v>2023</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
@@ -1439,7 +1453,7 @@
         <v>2023</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
@@ -1456,10 +1470,10 @@
         <v>2023</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E35">
         <v>3000000</v>
@@ -1473,10 +1487,10 @@
         <v>1961</v>
       </c>
       <c r="C36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E36">
         <v>62</v>
@@ -1490,10 +1504,10 @@
         <v>1961</v>
       </c>
       <c r="C37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E37">
         <v>80</v>
@@ -1507,10 +1521,10 @@
         <v>1961</v>
       </c>
       <c r="C38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E38">
         <v>150</v>
@@ -1524,10 +1538,10 @@
         <v>1961</v>
       </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E39">
         <v>19501008</v>
@@ -1541,10 +1555,10 @@
         <v>1961</v>
       </c>
       <c r="C40" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D40" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E40">
         <v>46.800000000000004</v>
@@ -1558,10 +1572,10 @@
         <v>1961</v>
       </c>
       <c r="C41" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D41" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E41">
         <v>10</v>
@@ -1575,10 +1589,10 @@
         <v>1961</v>
       </c>
       <c r="C42" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D42" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E42">
         <v>40</v>
@@ -1592,10 +1606,10 @@
         <v>1961</v>
       </c>
       <c r="C43" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D43" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E43">
         <v>30</v>
@@ -1609,10 +1623,10 @@
         <v>1961</v>
       </c>
       <c r="C44" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D44" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E44">
         <v>15</v>
@@ -1626,10 +1640,10 @@
         <v>1961</v>
       </c>
       <c r="C45" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D45" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E45">
         <v>0.5</v>
@@ -1643,10 +1657,10 @@
         <v>1961</v>
       </c>
       <c r="C46" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D46" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E46">
         <v>0.25</v>
@@ -1660,10 +1674,10 @@
         <v>1961</v>
       </c>
       <c r="C47" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D47" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E47">
         <v>2</v>
@@ -1677,10 +1691,10 @@
         <v>1961</v>
       </c>
       <c r="C48" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E48">
         <v>10</v>
@@ -1694,10 +1708,10 @@
         <v>1961</v>
       </c>
       <c r="C49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E49">
         <v>100</v>
@@ -1711,10 +1725,10 @@
         <v>1961</v>
       </c>
       <c r="C50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E50">
         <v>8603000</v>
@@ -1728,10 +1742,10 @@
         <v>1961</v>
       </c>
       <c r="C51" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D51" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E51">
         <v>35.880000000000003</v>
@@ -1745,10 +1759,10 @@
         <v>1961</v>
       </c>
       <c r="C52" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D52" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E52">
         <v>46.800000000000004</v>
@@ -1762,10 +1776,10 @@
         <v>1961</v>
       </c>
       <c r="C53" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D53" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E53">
         <v>10</v>
@@ -1779,10 +1793,10 @@
         <v>1961</v>
       </c>
       <c r="C54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D54" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E54">
         <v>35</v>
@@ -1796,10 +1810,10 @@
         <v>1961</v>
       </c>
       <c r="C55" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D55" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E55">
         <v>25</v>
@@ -1813,10 +1827,10 @@
         <v>1961</v>
       </c>
       <c r="C56" t="s">
+        <v>68</v>
+      </c>
+      <c r="D56" t="s">
         <v>71</v>
-      </c>
-      <c r="D56" t="s">
-        <v>74</v>
       </c>
       <c r="E56">
         <v>30</v>
@@ -1830,10 +1844,10 @@
         <v>1961</v>
       </c>
       <c r="C57" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D57" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E57">
         <v>4</v>
@@ -1847,10 +1861,10 @@
         <v>1961</v>
       </c>
       <c r="C58" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" t="s">
         <v>70</v>
-      </c>
-      <c r="D58" t="s">
-        <v>73</v>
       </c>
       <c r="E58">
         <v>0.2</v>
@@ -1864,10 +1878,10 @@
         <v>1961</v>
       </c>
       <c r="C59" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D59" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E59">
         <v>2</v>
@@ -1881,10 +1895,10 @@
         <v>2023</v>
       </c>
       <c r="C60" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E60">
         <v>70</v>
@@ -1898,10 +1912,10 @@
         <v>2023</v>
       </c>
       <c r="C61" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E61">
         <v>150</v>
@@ -1915,10 +1929,10 @@
         <v>2023</v>
       </c>
       <c r="C62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D62" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E62">
         <v>19501008</v>
@@ -1932,10 +1946,10 @@
         <v>2023</v>
       </c>
       <c r="C63" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" t="s">
         <v>66</v>
-      </c>
-      <c r="D63" t="s">
-        <v>69</v>
       </c>
       <c r="E63">
         <v>35.880000000000003</v>
@@ -1949,10 +1963,10 @@
         <v>2023</v>
       </c>
       <c r="C64" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D64" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E64">
         <v>46.800000000000004</v>
@@ -1966,10 +1980,10 @@
         <v>2023</v>
       </c>
       <c r="C65" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D65" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E65">
         <v>10</v>
@@ -1983,10 +1997,10 @@
         <v>2023</v>
       </c>
       <c r="C66" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D66" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E66">
         <v>2.5</v>
@@ -2000,10 +2014,10 @@
         <v>2023</v>
       </c>
       <c r="C67" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D67" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E67">
         <v>1.25</v>
@@ -2017,10 +2031,10 @@
         <v>2023</v>
       </c>
       <c r="C68" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D68" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E68">
         <v>10</v>
@@ -2034,10 +2048,10 @@
         <v>2023</v>
       </c>
       <c r="C69" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D69" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E69">
         <v>0.5</v>
@@ -2051,10 +2065,10 @@
         <v>2023</v>
       </c>
       <c r="C70" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D70" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E70">
         <v>0.25</v>
@@ -2068,10 +2082,10 @@
         <v>2023</v>
       </c>
       <c r="C71" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D71" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E71">
         <v>2</v>
@@ -2085,10 +2099,10 @@
         <v>2023</v>
       </c>
       <c r="C72" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D72" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E72">
         <v>20</v>
@@ -2102,10 +2116,10 @@
         <v>2023</v>
       </c>
       <c r="C73" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D73" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E73">
         <v>100</v>
@@ -2119,10 +2133,10 @@
         <v>2023</v>
       </c>
       <c r="C74" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D74" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E74">
         <v>8603000</v>
@@ -2136,10 +2150,10 @@
         <v>2023</v>
       </c>
       <c r="C75" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D75" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E75">
         <v>35.880000000000003</v>
@@ -2153,10 +2167,10 @@
         <v>2023</v>
       </c>
       <c r="C76" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D76" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E76">
         <v>46.800000000000004</v>
@@ -2170,10 +2184,10 @@
         <v>2023</v>
       </c>
       <c r="C77" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D77" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E77">
         <v>10</v>
@@ -2187,10 +2201,10 @@
         <v>2023</v>
       </c>
       <c r="C78" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D78" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E78">
         <v>28.999999999999996</v>
@@ -2204,10 +2218,10 @@
         <v>2023</v>
       </c>
       <c r="C79" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D79" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -2221,10 +2235,10 @@
         <v>2023</v>
       </c>
       <c r="C80" t="s">
+        <v>68</v>
+      </c>
+      <c r="D80" t="s">
         <v>71</v>
-      </c>
-      <c r="D80" t="s">
-        <v>74</v>
       </c>
       <c r="E80">
         <v>10</v>
@@ -2238,10 +2252,10 @@
         <v>2023</v>
       </c>
       <c r="C81" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D81" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E81">
         <v>4</v>
@@ -2255,10 +2269,10 @@
         <v>2023</v>
       </c>
       <c r="C82" t="s">
+        <v>67</v>
+      </c>
+      <c r="D82" t="s">
         <v>70</v>
-      </c>
-      <c r="D82" t="s">
-        <v>73</v>
       </c>
       <c r="E82">
         <v>0.2</v>
@@ -2272,10 +2286,10 @@
         <v>2023</v>
       </c>
       <c r="C83" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D83" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E83">
         <v>2</v>
@@ -2289,10 +2303,10 @@
         <v>1961</v>
       </c>
       <c r="C84" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D84" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E84">
         <v>40000000</v>
@@ -2306,10 +2320,10 @@
         <v>1961</v>
       </c>
       <c r="C85" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D85" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E85">
         <v>11.799999999999999</v>
@@ -2323,10 +2337,10 @@
         <v>1961</v>
       </c>
       <c r="C86" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D86" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E86">
         <v>42.5</v>
@@ -2340,10 +2354,10 @@
         <v>1961</v>
       </c>
       <c r="C87" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D87" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E87">
         <v>0.2</v>
@@ -2357,10 +2371,10 @@
         <v>1961</v>
       </c>
       <c r="C88" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D88" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E88">
         <v>6.5</v>
@@ -2374,10 +2388,10 @@
         <v>1961</v>
       </c>
       <c r="C89" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D89" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E89">
         <v>1.5</v>
@@ -2391,10 +2405,10 @@
         <v>1961</v>
       </c>
       <c r="C90" t="s">
+        <v>19</v>
+      </c>
+      <c r="D90" s="17" t="s">
         <v>20</v>
-      </c>
-      <c r="D90" s="17" t="s">
-        <v>21</v>
       </c>
       <c r="E90">
         <v>10</v>
@@ -2408,10 +2422,10 @@
         <v>2023</v>
       </c>
       <c r="C91" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D91" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E91">
         <v>70000000</v>
@@ -2425,10 +2439,10 @@
         <v>2023</v>
       </c>
       <c r="C92" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D92" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E92">
         <v>11.799999999999999</v>
@@ -2442,10 +2456,10 @@
         <v>2023</v>
       </c>
       <c r="C93" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D93" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E93">
         <v>42.5</v>
@@ -2459,10 +2473,10 @@
         <v>2023</v>
       </c>
       <c r="C94" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D94" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E94">
         <v>0.2</v>
@@ -2476,10 +2490,10 @@
         <v>2023</v>
       </c>
       <c r="C95" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D95" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E95">
         <v>6</v>
@@ -2493,10 +2507,10 @@
         <v>2023</v>
       </c>
       <c r="C96" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D96" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E96">
         <v>0.5</v>
@@ -2510,10 +2524,10 @@
         <v>2023</v>
       </c>
       <c r="C97" t="s">
+        <v>19</v>
+      </c>
+      <c r="D97" s="17" t="s">
         <v>20</v>
-      </c>
-      <c r="D97" s="17" t="s">
-        <v>21</v>
       </c>
       <c r="E97">
         <v>10</v>
@@ -2527,7 +2541,7 @@
         <v>1961</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>6</v>
@@ -2544,10 +2558,10 @@
         <v>1961</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E99" s="1">
         <v>40</v>
@@ -2561,7 +2575,7 @@
         <v>1961</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>7</v>
@@ -2578,7 +2592,7 @@
         <v>1961</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>8</v>
@@ -2595,7 +2609,7 @@
         <v>1961</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>9</v>
@@ -2612,7 +2626,7 @@
         <v>1961</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>11</v>
@@ -2629,10 +2643,10 @@
         <v>1961</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E104">
         <v>25</v>
@@ -2646,7 +2660,7 @@
         <v>2023</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>6</v>
@@ -2663,10 +2677,10 @@
         <v>2023</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E106" s="1">
         <v>40</v>
@@ -2680,7 +2694,7 @@
         <v>2023</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>7</v>
@@ -2697,7 +2711,7 @@
         <v>2023</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>8</v>
@@ -2714,7 +2728,7 @@
         <v>2023</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>9</v>
@@ -2731,7 +2745,7 @@
         <v>2023</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -2748,10 +2762,10 @@
         <v>2023</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E111">
         <v>25</v>
@@ -2765,7 +2779,7 @@
         <v>1961</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>6</v>
@@ -2782,10 +2796,10 @@
         <v>1961</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E113">
         <v>0.03</v>
@@ -2799,7 +2813,7 @@
         <v>1961</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>7</v>
@@ -2816,7 +2830,7 @@
         <v>1961</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>8</v>
@@ -2833,7 +2847,7 @@
         <v>1961</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>9</v>
@@ -2850,7 +2864,7 @@
         <v>1961</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>11</v>
@@ -2867,10 +2881,10 @@
         <v>1961</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E118">
         <v>0</v>
@@ -2884,7 +2898,7 @@
         <v>2023</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>6</v>
@@ -2901,10 +2915,10 @@
         <v>2023</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E120">
         <v>0.03</v>
@@ -2918,7 +2932,7 @@
         <v>2023</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>7</v>
@@ -2935,7 +2949,7 @@
         <v>2023</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>8</v>
@@ -2952,7 +2966,7 @@
         <v>2023</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>9</v>
@@ -2969,7 +2983,7 @@
         <v>2023</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>11</v>
@@ -2986,10 +3000,10 @@
         <v>2023</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E125">
         <v>0</v>
@@ -3000,16 +3014,16 @@
         <v>5</v>
       </c>
       <c r="B126">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E126">
-        <v>100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
@@ -3017,16 +3031,16 @@
         <v>5</v>
       </c>
       <c r="B127">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E127">
-        <v>300</v>
+        <v>50</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
@@ -3034,16 +3048,16 @@
         <v>5</v>
       </c>
       <c r="B128">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E128">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
@@ -3051,16 +3065,16 @@
         <v>5</v>
       </c>
       <c r="B129">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E129">
-        <v>70</v>
+        <v>8</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
@@ -3068,13 +3082,13 @@
         <v>5</v>
       </c>
       <c r="B130">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E130">
         <v>8</v>
@@ -3088,13 +3102,13 @@
         <v>2023</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E131">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
@@ -3105,13 +3119,13 @@
         <v>2023</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E132">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
@@ -3122,13 +3136,13 @@
         <v>2023</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E133">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
@@ -3136,16 +3150,16 @@
         <v>5</v>
       </c>
       <c r="B134">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E134">
-        <v>0.05</v>
+        <v>58</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
@@ -3153,16 +3167,16 @@
         <v>5</v>
       </c>
       <c r="B135">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
@@ -3173,13 +3187,13 @@
         <v>2023</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>63</v>
+        <v>24</v>
+      </c>
+      <c r="D136" t="s">
+        <v>13</v>
+      </c>
+      <c r="E136" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
@@ -3190,7 +3204,7 @@
         <v>2023</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D137" t="s">
         <v>14</v>
@@ -3207,10 +3221,10 @@
         <v>2023</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D138" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E138" t="s">
         <v>27</v>
@@ -3221,16 +3235,16 @@
         <v>5</v>
       </c>
       <c r="B139">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D139" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E139" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
@@ -3241,7 +3255,7 @@
         <v>1961</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D140" t="s">
         <v>14</v>
@@ -3258,30 +3272,30 @@
         <v>1961</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D141" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E141" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A142" s="1" t="s">
+      <c r="A142" t="s">
         <v>5</v>
       </c>
       <c r="B142">
         <v>1961</v>
       </c>
-      <c r="C142" s="1" t="s">
-        <v>25</v>
+      <c r="C142" t="s">
+        <v>24</v>
       </c>
       <c r="D142" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="E142" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
@@ -3289,168 +3303,168 @@
         <v>5</v>
       </c>
       <c r="B143">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C143" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D143" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E143" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
-        <v>5</v>
-      </c>
-      <c r="B144">
-        <v>2023</v>
-      </c>
-      <c r="C144" t="s">
-        <v>25</v>
-      </c>
-      <c r="D144" t="s">
-        <v>80</v>
-      </c>
-      <c r="E144" t="s">
-        <v>76</v>
+      <c r="A144" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B144" s="2">
+        <v>1961</v>
+      </c>
+      <c r="C144" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D144" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E144" s="8">
+        <v>2.76</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A145" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B145" s="2">
-        <v>1961</v>
-      </c>
-      <c r="C145" s="5" t="s">
+      <c r="A145" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B145" s="3">
+        <v>1961</v>
+      </c>
+      <c r="C145" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D145" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E145" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A146" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B146" s="2">
+        <v>1961</v>
+      </c>
+      <c r="C146" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D145" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E145" s="8">
-        <v>2.76</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A146" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B146" s="3">
-        <v>1961</v>
-      </c>
-      <c r="C146" s="6" t="s">
+      <c r="D146" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E146" s="8">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A147" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B147" s="3">
+        <v>1961</v>
+      </c>
+      <c r="C147" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D146" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E146" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A147" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B147" s="2">
-        <v>1961</v>
-      </c>
-      <c r="C147" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D147" s="5" t="s">
-        <v>6</v>
+      <c r="D147" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="E147" s="8">
-        <v>2.5</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A148" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B148" s="3">
+      <c r="A148" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B148" s="2">
         <v>1961</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D148" s="6" t="s">
-        <v>58</v>
+        <v>32</v>
+      </c>
+      <c r="D148" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="E148" s="8">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A149" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B149" s="2">
+      <c r="A149" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B149" s="3">
         <v>1961</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D149" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E149" s="8">
-        <v>2.2000000000000002</v>
+        <v>32</v>
+      </c>
+      <c r="D149" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E149" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A150" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B150" s="3">
+      <c r="A150" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B150" s="2">
         <v>1961</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D150" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E150" s="4">
+        <v>32</v>
+      </c>
+      <c r="D150" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E150" s="8">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A151" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B151" s="3">
+        <v>1961</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D151" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E151" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A151" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B151" s="2">
-        <v>1961</v>
-      </c>
-      <c r="C151" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D151" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E151" s="8">
-        <v>3.5</v>
-      </c>
-    </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A152" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B152" s="3">
+      <c r="A152" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B152" s="2">
         <v>1961</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D152" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E152" s="11">
+        <v>32</v>
+      </c>
+      <c r="D152" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E152" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3459,117 +3473,117 @@
         <v>5</v>
       </c>
       <c r="B153" s="2">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D153" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E153" s="12">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="E153" s="8">
+        <v>2.5</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A154" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B154" s="2">
+      <c r="A154" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B154" s="3">
         <v>2023</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D154" s="5" t="s">
-        <v>6</v>
+        <v>32</v>
+      </c>
+      <c r="D154" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="E154" s="8">
-        <v>2.5</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A155" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B155" s="3">
+      <c r="A155" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B155" s="2">
         <v>2023</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D155" s="6" t="s">
-        <v>58</v>
+        <v>32</v>
+      </c>
+      <c r="D155" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="E155" s="8">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A156" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B156" s="2">
+      <c r="A156" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B156" s="3">
         <v>2023</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D156" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E156" s="8">
-        <v>2.2000000000000002</v>
+        <v>32</v>
+      </c>
+      <c r="D156" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E156" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A157" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B157" s="3">
+      <c r="A157" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B157" s="2">
         <v>2023</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D157" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E157" s="4">
+        <v>32</v>
+      </c>
+      <c r="D157" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E157" s="8">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A158" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B158" s="3">
+        <v>2023</v>
+      </c>
+      <c r="C158" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D158" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E158" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A158" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B158" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C158" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D158" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E158" s="8">
-        <v>3.5</v>
-      </c>
-    </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A159" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B159" s="3">
+      <c r="A159" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B159" s="2">
         <v>2023</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D159" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E159" s="11">
+        <v>32</v>
+      </c>
+      <c r="D159" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E159" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3578,118 +3592,118 @@
         <v>5</v>
       </c>
       <c r="B160" s="2">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C160" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D160" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E160" s="12">
+        <v>6</v>
+      </c>
+      <c r="E160">
         <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A161" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B161" s="2">
+      <c r="A161" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B161" s="3">
         <v>1961</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D161" s="5" t="s">
-        <v>6</v>
+        <v>33</v>
+      </c>
+      <c r="D161" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="E161">
         <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A162" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B162" s="3">
+      <c r="A162" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B162" s="2">
         <v>1961</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D162" s="6" t="s">
-        <v>58</v>
+        <v>33</v>
+      </c>
+      <c r="D162" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="E162">
         <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A163" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B163" s="2">
+      <c r="A163" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B163" s="3">
         <v>1961</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D163" s="5" t="s">
-        <v>7</v>
+        <v>33</v>
+      </c>
+      <c r="D163" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E163">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A164" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B164" s="2">
+        <v>1961</v>
+      </c>
+      <c r="C164" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D164" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E164">
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A164" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B164" s="3">
-        <v>1961</v>
-      </c>
-      <c r="C164" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D164" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E164">
-        <v>125</v>
-      </c>
-    </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A165" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B165" s="2">
+      <c r="A165" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B165" s="3">
         <v>1961</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D165" s="5" t="s">
-        <v>9</v>
+        <v>33</v>
+      </c>
+      <c r="D165" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E165">
         <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A166" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B166" s="3">
+      <c r="A166" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B166" s="2">
         <v>1961</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D166" s="6" t="s">
-        <v>11</v>
+        <v>33</v>
+      </c>
+      <c r="D166" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="E166">
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.35">
@@ -3697,170 +3711,739 @@
         <v>5</v>
       </c>
       <c r="B167" s="2">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D167" s="5" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E167">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A168" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B168" s="2">
+      <c r="A168" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B168" s="3">
         <v>2023</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D168" s="5" t="s">
-        <v>6</v>
+        <v>33</v>
+      </c>
+      <c r="D168" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="E168">
         <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A169" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B169" s="3">
+      <c r="A169" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B169" s="2">
         <v>2023</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D169" s="6" t="s">
-        <v>58</v>
+        <v>33</v>
+      </c>
+      <c r="D169" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="E169">
         <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A170" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B170" s="2">
+      <c r="A170" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B170" s="3">
         <v>2023</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D170" s="5" t="s">
-        <v>7</v>
+        <v>33</v>
+      </c>
+      <c r="D170" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E170">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A171" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B171" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C171" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D171" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E171">
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A171" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B171" s="3">
-        <v>2023</v>
-      </c>
-      <c r="C171" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D171" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E171">
-        <v>125</v>
-      </c>
-    </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A172" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B172" s="2">
+      <c r="A172" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B172" s="3">
         <v>2023</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D172" s="5" t="s">
-        <v>9</v>
+        <v>33</v>
+      </c>
+      <c r="D172" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E172">
         <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A173" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B173" s="3">
+      <c r="A173" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B173" s="2">
         <v>2023</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D173" s="6" t="s">
-        <v>11</v>
+        <v>33</v>
+      </c>
+      <c r="D173" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="E173">
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A174" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B174" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C174" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D174" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E174">
-        <v>150</v>
+      <c r="A174" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B174">
+        <v>1961</v>
+      </c>
+      <c r="C174" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D174" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E174" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A175" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B175" s="14">
-        <v>1961</v>
-      </c>
-      <c r="C175" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D175" t="s">
-        <v>39</v>
-      </c>
-      <c r="E175">
-        <v>20</v>
+      <c r="A175" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B175" s="21">
+        <v>2023</v>
+      </c>
+      <c r="C175" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D175" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E175" s="24">
+        <v>25</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A176" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B176" s="14">
-        <v>2023</v>
-      </c>
-      <c r="C176" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D176" t="s">
-        <v>39</v>
-      </c>
-      <c r="E176">
-        <v>25</v>
-      </c>
+      <c r="A176" s="10"/>
+      <c r="B176" s="3"/>
+      <c r="C176" s="5"/>
+      <c r="D176" s="6"/>
+      <c r="E176" s="4"/>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A177" s="9"/>
+      <c r="B177" s="2"/>
+      <c r="C177" s="5"/>
+      <c r="D177" s="5"/>
+      <c r="E177" s="8"/>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A178" s="10"/>
+      <c r="B178" s="3"/>
+      <c r="C178" s="5"/>
+      <c r="D178" s="6"/>
+      <c r="E178" s="11"/>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A179" s="9"/>
+      <c r="B179" s="2"/>
+      <c r="C179" s="5"/>
+      <c r="D179" s="5"/>
+      <c r="E179" s="12"/>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A180" s="9"/>
+      <c r="B180" s="2"/>
+      <c r="C180" s="5"/>
+      <c r="D180" s="5"/>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A181" s="10"/>
+      <c r="B181" s="3"/>
+      <c r="C181" s="5"/>
+      <c r="D181" s="6"/>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A182" s="9"/>
+      <c r="B182" s="2"/>
+      <c r="C182" s="5"/>
+      <c r="D182" s="5"/>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A183" s="10"/>
+      <c r="B183" s="3"/>
+      <c r="C183" s="5"/>
+      <c r="D183" s="6"/>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A184" s="9"/>
+      <c r="B184" s="2"/>
+      <c r="C184" s="5"/>
+      <c r="D184" s="5"/>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A185" s="10"/>
+      <c r="B185" s="3"/>
+      <c r="C185" s="5"/>
+      <c r="D185" s="6"/>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A186" s="9"/>
+      <c r="B186" s="2"/>
+      <c r="C186" s="5"/>
+      <c r="D186" s="5"/>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A187" s="9"/>
+      <c r="B187" s="2"/>
+      <c r="C187" s="5"/>
+      <c r="D187" s="5"/>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A188" s="10"/>
+      <c r="B188" s="3"/>
+      <c r="C188" s="5"/>
+      <c r="D188" s="6"/>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A189" s="9"/>
+      <c r="B189" s="2"/>
+      <c r="C189" s="5"/>
+      <c r="D189" s="5"/>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A190" s="10"/>
+      <c r="B190" s="3"/>
+      <c r="C190" s="5"/>
+      <c r="D190" s="6"/>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A191" s="9"/>
+      <c r="B191" s="2"/>
+      <c r="C191" s="5"/>
+      <c r="D191" s="5"/>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A192" s="10"/>
+      <c r="B192" s="3"/>
+      <c r="C192" s="5"/>
+      <c r="D192" s="6"/>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A193" s="9"/>
+      <c r="B193" s="2"/>
+      <c r="C193" s="5"/>
+      <c r="D193" s="5"/>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A194" s="13"/>
+      <c r="B194" s="14"/>
+      <c r="C194" s="15"/>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A195" s="13"/>
+      <c r="B195" s="14"/>
+      <c r="C195" s="15"/>
+    </row>
+    <row r="264" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D264" s="16"/>
+    </row>
+    <row r="265" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D265" s="17"/>
+    </row>
+    <row r="266" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D266" s="16"/>
+    </row>
+    <row r="267" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D267" s="17"/>
+    </row>
+    <row r="268" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D268" s="16"/>
+    </row>
+    <row r="269" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D269" s="17"/>
+    </row>
+    <row r="270" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D270" s="17"/>
+    </row>
+    <row r="271" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D271" s="16"/>
+    </row>
+    <row r="272" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D272" s="17"/>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D273" s="16"/>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D274" s="17"/>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D275" s="16"/>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D276" s="17"/>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D277" s="17"/>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A278" s="1"/>
+      <c r="C278" s="1"/>
+      <c r="D278" s="1"/>
+      <c r="E278" s="1"/>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A279" s="1"/>
+      <c r="C279" s="1"/>
+      <c r="D279" s="1"/>
+      <c r="E279" s="1"/>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A280" s="1"/>
+      <c r="C280" s="1"/>
+      <c r="D280" s="1"/>
+      <c r="E280" s="1"/>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A281" s="1"/>
+      <c r="C281" s="1"/>
+      <c r="D281" s="1"/>
+      <c r="E281" s="1"/>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A282" s="1"/>
+      <c r="C282" s="1"/>
+      <c r="D282" s="1"/>
+      <c r="E282" s="1"/>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A283" s="1"/>
+      <c r="C283" s="1"/>
+      <c r="D283" s="1"/>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A284" s="1"/>
+      <c r="C284" s="1"/>
+      <c r="D284" s="1"/>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A285" s="1"/>
+      <c r="C285" s="1"/>
+      <c r="D285" s="1"/>
+      <c r="E285" s="1"/>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A286" s="1"/>
+      <c r="C286" s="1"/>
+      <c r="D286" s="1"/>
+      <c r="E286" s="1"/>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A287" s="1"/>
+      <c r="C287" s="1"/>
+      <c r="D287" s="1"/>
+      <c r="E287" s="1"/>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A288" s="1"/>
+      <c r="C288" s="1"/>
+      <c r="D288" s="1"/>
+      <c r="E288" s="1"/>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A289" s="1"/>
+      <c r="C289" s="1"/>
+      <c r="D289" s="1"/>
+      <c r="E289" s="1"/>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A290" s="1"/>
+      <c r="C290" s="1"/>
+      <c r="D290" s="1"/>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A291" s="1"/>
+      <c r="C291" s="1"/>
+      <c r="D291" s="1"/>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A292" s="1"/>
+      <c r="C292" s="1"/>
+      <c r="D292" s="1"/>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A293" s="1"/>
+      <c r="C293" s="1"/>
+      <c r="D293" s="1"/>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A294" s="1"/>
+      <c r="C294" s="1"/>
+      <c r="D294" s="1"/>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A295" s="1"/>
+      <c r="C295" s="1"/>
+      <c r="D295" s="1"/>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A296" s="1"/>
+      <c r="C296" s="1"/>
+      <c r="D296" s="1"/>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A297" s="1"/>
+      <c r="C297" s="1"/>
+      <c r="D297" s="1"/>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A298" s="1"/>
+      <c r="C298" s="1"/>
+      <c r="D298" s="1"/>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A299" s="1"/>
+      <c r="C299" s="1"/>
+      <c r="D299" s="1"/>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A300" s="1"/>
+      <c r="C300" s="1"/>
+      <c r="D300" s="1"/>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A301" s="1"/>
+      <c r="C301" s="1"/>
+      <c r="D301" s="1"/>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A302" s="1"/>
+      <c r="C302" s="1"/>
+      <c r="D302" s="1"/>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A303" s="1"/>
+      <c r="C303" s="1"/>
+      <c r="D303" s="1"/>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A304" s="1"/>
+      <c r="C304" s="1"/>
+      <c r="D304" s="1"/>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A305" s="1"/>
+      <c r="C305" s="1"/>
+      <c r="D305" s="1"/>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A306" s="1"/>
+      <c r="C306" s="1"/>
+      <c r="D306" s="1"/>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A307" s="1"/>
+      <c r="C307" s="1"/>
+      <c r="D307" s="1"/>
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A308" s="1"/>
+      <c r="C308" s="1"/>
+      <c r="D308" s="1"/>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A309" s="1"/>
+      <c r="C309" s="1"/>
+      <c r="D309" s="1"/>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A310" s="1"/>
+      <c r="C310" s="1"/>
+      <c r="D310" s="1"/>
+    </row>
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A311" s="1"/>
+      <c r="C311" s="1"/>
+      <c r="D311" s="1"/>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A312" s="1"/>
+      <c r="C312" s="1"/>
+      <c r="D312" s="1"/>
+    </row>
+    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A313" s="1"/>
+      <c r="C313" s="1"/>
+      <c r="D313" s="1"/>
+    </row>
+    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A314" s="1"/>
+      <c r="C314" s="1"/>
+      <c r="D314" s="1"/>
+      <c r="E314" s="1"/>
+    </row>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A315" s="1"/>
+      <c r="C315" s="1"/>
+      <c r="D315" s="1"/>
+      <c r="E315" s="1"/>
+    </row>
+    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A316" s="1"/>
+      <c r="C316" s="1"/>
+    </row>
+    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A317" s="1"/>
+      <c r="C317" s="1"/>
+    </row>
+    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A318" s="1"/>
+      <c r="C318" s="1"/>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A319" s="1"/>
+      <c r="C319" s="1"/>
+    </row>
+    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A320" s="1"/>
+      <c r="C320" s="1"/>
+    </row>
+    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A321" s="1"/>
+      <c r="C321" s="1"/>
+    </row>
+    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A324" s="9"/>
+      <c r="B324" s="2"/>
+      <c r="C324" s="5"/>
+      <c r="D324" s="5"/>
+      <c r="E324" s="8"/>
+    </row>
+    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A325" s="10"/>
+      <c r="B325" s="3"/>
+      <c r="C325" s="6"/>
+      <c r="D325" s="6"/>
+      <c r="E325" s="8"/>
+    </row>
+    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A326" s="9"/>
+      <c r="B326" s="2"/>
+      <c r="C326" s="5"/>
+      <c r="D326" s="5"/>
+      <c r="E326" s="8"/>
+    </row>
+    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A327" s="10"/>
+      <c r="B327" s="3"/>
+      <c r="C327" s="5"/>
+      <c r="D327" s="6"/>
+      <c r="E327" s="8"/>
+    </row>
+    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A328" s="9"/>
+      <c r="B328" s="2"/>
+      <c r="C328" s="5"/>
+      <c r="D328" s="5"/>
+      <c r="E328" s="8"/>
+    </row>
+    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A329" s="10"/>
+      <c r="B329" s="3"/>
+      <c r="C329" s="5"/>
+      <c r="D329" s="6"/>
+      <c r="E329" s="4"/>
+    </row>
+    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A330" s="9"/>
+      <c r="B330" s="2"/>
+      <c r="C330" s="5"/>
+      <c r="D330" s="5"/>
+      <c r="E330" s="8"/>
+    </row>
+    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A331" s="10"/>
+      <c r="B331" s="3"/>
+      <c r="C331" s="5"/>
+      <c r="D331" s="6"/>
+      <c r="E331" s="11"/>
+    </row>
+    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A332" s="9"/>
+      <c r="B332" s="2"/>
+      <c r="C332" s="5"/>
+      <c r="D332" s="5"/>
+      <c r="E332" s="12"/>
+    </row>
+    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A333" s="9"/>
+      <c r="B333" s="2"/>
+      <c r="C333" s="5"/>
+      <c r="D333" s="5"/>
+      <c r="E333" s="8"/>
+    </row>
+    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A334" s="10"/>
+      <c r="B334" s="3"/>
+      <c r="C334" s="5"/>
+      <c r="D334" s="6"/>
+      <c r="E334" s="8"/>
+    </row>
+    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A335" s="9"/>
+      <c r="B335" s="2"/>
+      <c r="C335" s="5"/>
+      <c r="D335" s="5"/>
+      <c r="E335" s="8"/>
+    </row>
+    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A336" s="10"/>
+      <c r="B336" s="3"/>
+      <c r="C336" s="5"/>
+      <c r="D336" s="6"/>
+      <c r="E336" s="4"/>
+    </row>
+    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A337" s="9"/>
+      <c r="B337" s="2"/>
+      <c r="C337" s="5"/>
+      <c r="D337" s="5"/>
+      <c r="E337" s="8"/>
+    </row>
+    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A338" s="10"/>
+      <c r="B338" s="3"/>
+      <c r="C338" s="5"/>
+      <c r="D338" s="6"/>
+      <c r="E338" s="11"/>
+    </row>
+    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A339" s="9"/>
+      <c r="B339" s="2"/>
+      <c r="C339" s="5"/>
+      <c r="D339" s="5"/>
+      <c r="E339" s="12"/>
+    </row>
+    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A340" s="9"/>
+      <c r="B340" s="2"/>
+      <c r="C340" s="5"/>
+      <c r="D340" s="5"/>
+    </row>
+    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A341" s="10"/>
+      <c r="B341" s="3"/>
+      <c r="C341" s="5"/>
+      <c r="D341" s="6"/>
+    </row>
+    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A342" s="9"/>
+      <c r="B342" s="2"/>
+      <c r="C342" s="5"/>
+      <c r="D342" s="5"/>
+    </row>
+    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A343" s="10"/>
+      <c r="B343" s="3"/>
+      <c r="C343" s="5"/>
+      <c r="D343" s="6"/>
+    </row>
+    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A344" s="9"/>
+      <c r="B344" s="2"/>
+      <c r="C344" s="5"/>
+      <c r="D344" s="5"/>
+    </row>
+    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A345" s="10"/>
+      <c r="B345" s="3"/>
+      <c r="C345" s="5"/>
+      <c r="D345" s="6"/>
+    </row>
+    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A346" s="9"/>
+      <c r="B346" s="2"/>
+      <c r="C346" s="5"/>
+      <c r="D346" s="5"/>
+    </row>
+    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A347" s="9"/>
+      <c r="B347" s="2"/>
+      <c r="C347" s="5"/>
+      <c r="D347" s="5"/>
+    </row>
+    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A348" s="10"/>
+      <c r="B348" s="3"/>
+      <c r="C348" s="5"/>
+      <c r="D348" s="6"/>
+    </row>
+    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A349" s="9"/>
+      <c r="B349" s="2"/>
+      <c r="C349" s="5"/>
+      <c r="D349" s="5"/>
+    </row>
+    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A350" s="10"/>
+      <c r="B350" s="3"/>
+      <c r="C350" s="5"/>
+      <c r="D350" s="6"/>
+    </row>
+    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A351" s="9"/>
+      <c r="B351" s="2"/>
+      <c r="C351" s="5"/>
+      <c r="D351" s="5"/>
+    </row>
+    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A352" s="10"/>
+      <c r="B352" s="3"/>
+      <c r="C352" s="5"/>
+      <c r="D352" s="6"/>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A353" s="9"/>
+      <c r="B353" s="2"/>
+      <c r="C353" s="5"/>
+      <c r="D353" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3887,315 +4470,315 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>0.65</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>0.1</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>0.25</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5">
         <v>0.3</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>0.1</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>0.2</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8">
         <v>0.4</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9">
         <v>0.6</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>0.1</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>0.05</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12">
         <v>0.1</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13">
         <v>0.05</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14">
         <v>0.1</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>0.5</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16">
         <v>0.3</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17">
         <v>0.2</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18">
         <v>0.3</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19">
         <v>0.1</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20">
         <v>0.2</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21">
         <v>0.4</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22">
         <v>0.3</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23">
         <v>0.05</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25">
         <v>0.05</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27">
         <v>0.05</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28">
         <v>0.3</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29">
         <v>0.05</v>
@@ -4206,79 +4789,79 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30">
         <v>0.15</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B31">
         <v>0.2</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B32">
         <v>0.1</v>
       </c>
       <c r="C32" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B33">
         <v>0.6</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B34">
         <v>0.1</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B35">
         <v>0.5</v>
       </c>
       <c r="C35" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B36">
         <v>0.5</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -4302,21 +4885,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
         <v>84</v>
-      </c>
-      <c r="B1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C2">
         <v>0.78</v>
@@ -4324,10 +4907,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C3">
         <v>0.5</v>
@@ -4335,10 +4918,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C4">
         <v>0.23</v>
@@ -4346,10 +4929,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C5">
         <v>0.25</v>
@@ -4357,10 +4940,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C6">
         <v>0.1</v>
@@ -4368,10 +4951,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C7">
         <v>0.1</v>

</xml_diff>